<commit_message>
Asignación de vuelos OFF (Falta considerar casos de TBC)
</commit_message>
<xml_diff>
--- a/ejemplo_carga_masiva.xlsx
+++ b/ejemplo_carga_masiva.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2432" uniqueCount="668">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2429" uniqueCount="666">
   <si>
     <t xml:space="preserve">Owner</t>
   </si>
@@ -1391,9 +1391,6 @@
     <t xml:space="preserve">F36071497</t>
   </si>
   <si>
-    <t xml:space="preserve">NO</t>
-  </si>
-  <si>
     <t xml:space="preserve">CHEN</t>
   </si>
   <si>
@@ -1946,18 +1943,18 @@
     <t xml:space="preserve">LATAM AIRLINES</t>
   </si>
   <si>
+    <t xml:space="preserve">LA310 PUQ-SCL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12:00-16:30+1</t>
+  </si>
+  <si>
     <t xml:space="preserve">OU651 SPU-ZAG</t>
   </si>
   <si>
     <t xml:space="preserve">06:50-07:40</t>
   </si>
   <si>
-    <t xml:space="preserve">LA310 PUQ-SCL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12:00-16:30+1</t>
-  </si>
-  <si>
     <t xml:space="preserve">Hotel SCL</t>
   </si>
   <si>
@@ -2015,10 +2012,7 @@
     <t xml:space="preserve">10/22/1986</t>
   </si>
   <si>
-    <t xml:space="preserve">KL702 SCL-AMS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10:50-12:00</t>
+    <t xml:space="preserve">15:00-17:03+1</t>
   </si>
   <si>
     <t xml:space="preserve">10:17-15:05</t>
@@ -2587,8 +2581,8 @@
   </sheetPr>
   <dimension ref="A1:CH75"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AG1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AM5" activeCellId="0" sqref="AM5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11530,15 +11524,9 @@
       <c r="AM47" s="32"/>
       <c r="AN47" s="33"/>
       <c r="AO47" s="32"/>
-      <c r="AP47" s="32" t="s">
-        <v>456</v>
-      </c>
-      <c r="AQ47" s="32" t="s">
-        <v>456</v>
-      </c>
-      <c r="AR47" s="32" t="s">
-        <v>456</v>
-      </c>
+      <c r="AP47" s="32"/>
+      <c r="AQ47" s="32"/>
+      <c r="AR47" s="32"/>
       <c r="AS47" s="32"/>
       <c r="AT47" s="32"/>
       <c r="AU47" s="33"/>
@@ -11604,22 +11592,22 @@
       <c r="H48" s="32"/>
       <c r="I48" s="32"/>
       <c r="J48" s="32" t="s">
+        <v>456</v>
+      </c>
+      <c r="K48" s="32" t="s">
         <v>457</v>
-      </c>
-      <c r="K48" s="32" t="s">
-        <v>458</v>
       </c>
       <c r="L48" s="32" t="s">
         <v>128</v>
       </c>
       <c r="M48" s="32" t="s">
+        <v>458</v>
+      </c>
+      <c r="N48" s="32" t="s">
         <v>459</v>
       </c>
-      <c r="N48" s="32" t="s">
+      <c r="O48" s="32" t="s">
         <v>460</v>
-      </c>
-      <c r="O48" s="32" t="s">
-        <v>461</v>
       </c>
       <c r="P48" s="33" t="n">
         <v>33808</v>
@@ -11637,22 +11625,22 @@
         <v>98</v>
       </c>
       <c r="U48" s="32" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="V48" s="33" t="n">
         <v>45609</v>
       </c>
       <c r="W48" s="33" t="s">
+        <v>462</v>
+      </c>
+      <c r="X48" s="32" t="s">
         <v>463</v>
-      </c>
-      <c r="X48" s="32" t="s">
-        <v>464</v>
       </c>
       <c r="Y48" s="33" t="n">
         <v>45609</v>
       </c>
       <c r="Z48" s="33" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="AA48" s="32"/>
       <c r="AB48" s="33"/>
@@ -11661,7 +11649,7 @@
       <c r="AE48" s="32"/>
       <c r="AF48" s="32"/>
       <c r="AG48" s="32" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="AH48" s="33" t="n">
         <v>45609</v>
@@ -11670,7 +11658,7 @@
         <v>168</v>
       </c>
       <c r="AJ48" s="32" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="AK48" s="33" t="n">
         <v>45656</v>
@@ -11679,7 +11667,7 @@
         <v>168</v>
       </c>
       <c r="AM48" s="32" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="AN48" s="33" t="n">
         <v>45615</v>
@@ -11761,10 +11749,10 @@
       <c r="H49" s="32"/>
       <c r="I49" s="32"/>
       <c r="J49" s="32" t="s">
+        <v>467</v>
+      </c>
+      <c r="K49" s="32" t="s">
         <v>468</v>
-      </c>
-      <c r="K49" s="32" t="s">
-        <v>469</v>
       </c>
       <c r="L49" s="32" t="s">
         <v>128</v>
@@ -11773,10 +11761,10 @@
         <v>174</v>
       </c>
       <c r="N49" s="32" t="s">
+        <v>469</v>
+      </c>
+      <c r="O49" s="32" t="s">
         <v>470</v>
-      </c>
-      <c r="O49" s="32" t="s">
-        <v>471</v>
       </c>
       <c r="P49" s="33" t="n">
         <v>36243</v>
@@ -11794,7 +11782,7 @@
         <v>98</v>
       </c>
       <c r="U49" s="32" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="V49" s="33"/>
       <c r="W49" s="33"/>
@@ -11808,7 +11796,7 @@
       <c r="AE49" s="32"/>
       <c r="AF49" s="32"/>
       <c r="AG49" s="32" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="AH49" s="33" t="s">
         <v>98</v>
@@ -11824,13 +11812,13 @@
         <v>98</v>
       </c>
       <c r="AM49" s="32" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="AN49" s="33" t="n">
         <v>45615</v>
       </c>
       <c r="AO49" s="32" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="AP49" s="32" t="s">
         <v>109</v>
@@ -11906,10 +11894,10 @@
       <c r="H50" s="32"/>
       <c r="I50" s="32"/>
       <c r="J50" s="32" t="s">
+        <v>473</v>
+      </c>
+      <c r="K50" s="32" t="s">
         <v>474</v>
-      </c>
-      <c r="K50" s="32" t="s">
-        <v>475</v>
       </c>
       <c r="L50" s="32" t="s">
         <v>128</v>
@@ -11918,10 +11906,10 @@
         <v>249</v>
       </c>
       <c r="N50" s="32" t="s">
+        <v>475</v>
+      </c>
+      <c r="O50" s="32" t="s">
         <v>476</v>
-      </c>
-      <c r="O50" s="32" t="s">
-        <v>477</v>
       </c>
       <c r="P50" s="33" t="n">
         <v>34162</v>
@@ -11939,16 +11927,16 @@
         <v>98</v>
       </c>
       <c r="U50" s="32" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="V50" s="33" t="n">
         <v>45613</v>
       </c>
       <c r="W50" s="33" t="s">
+        <v>478</v>
+      </c>
+      <c r="X50" s="32" t="s">
         <v>479</v>
-      </c>
-      <c r="X50" s="32" t="s">
-        <v>480</v>
       </c>
       <c r="Y50" s="33" t="n">
         <v>45613</v>
@@ -11957,43 +11945,43 @@
         <v>102</v>
       </c>
       <c r="AA50" s="32" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="AB50" s="33" t="n">
         <v>45613</v>
       </c>
       <c r="AC50" s="33" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="AD50" s="32"/>
       <c r="AE50" s="32"/>
       <c r="AF50" s="32"/>
       <c r="AG50" s="32" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="AH50" s="33" t="n">
         <v>45613</v>
       </c>
       <c r="AI50" s="32" t="s">
+        <v>482</v>
+      </c>
+      <c r="AJ50" s="32" t="s">
         <v>483</v>
-      </c>
-      <c r="AJ50" s="32" t="s">
-        <v>484</v>
       </c>
       <c r="AK50" s="33" t="n">
         <v>45658</v>
       </c>
       <c r="AL50" s="32" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="AM50" s="32" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="AN50" s="33" t="n">
         <v>45615</v>
       </c>
       <c r="AO50" s="32" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="AP50" s="32" t="s">
         <v>109</v>
@@ -12069,10 +12057,10 @@
       <c r="H51" s="32"/>
       <c r="I51" s="32"/>
       <c r="J51" s="32" t="s">
+        <v>485</v>
+      </c>
+      <c r="K51" s="32" t="s">
         <v>486</v>
-      </c>
-      <c r="K51" s="32" t="s">
-        <v>487</v>
       </c>
       <c r="L51" s="32" t="s">
         <v>128</v>
@@ -12081,10 +12069,10 @@
         <v>249</v>
       </c>
       <c r="N51" s="32" t="s">
+        <v>487</v>
+      </c>
+      <c r="O51" s="32" t="s">
         <v>488</v>
-      </c>
-      <c r="O51" s="32" t="s">
-        <v>489</v>
       </c>
       <c r="P51" s="33" t="n">
         <v>27249</v>
@@ -12102,7 +12090,7 @@
         <v>98</v>
       </c>
       <c r="U51" s="32" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="V51" s="33"/>
       <c r="W51" s="33"/>
@@ -12116,31 +12104,31 @@
       <c r="AE51" s="32"/>
       <c r="AF51" s="32"/>
       <c r="AG51" s="32" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="AH51" s="33" t="s">
         <v>98</v>
       </c>
       <c r="AI51" s="32" t="s">
+        <v>489</v>
+      </c>
+      <c r="AJ51" s="32" t="s">
         <v>490</v>
-      </c>
-      <c r="AJ51" s="32" t="s">
-        <v>491</v>
       </c>
       <c r="AK51" s="33" t="n">
         <v>45659</v>
       </c>
       <c r="AL51" s="32" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="AM51" s="32" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="AN51" s="33" t="n">
         <v>45615</v>
       </c>
       <c r="AO51" s="32" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="AP51" s="32" t="s">
         <v>109</v>
@@ -12216,10 +12204,10 @@
       <c r="H52" s="32"/>
       <c r="I52" s="32"/>
       <c r="J52" s="32" t="s">
+        <v>492</v>
+      </c>
+      <c r="K52" s="32" t="s">
         <v>493</v>
-      </c>
-      <c r="K52" s="32" t="s">
-        <v>494</v>
       </c>
       <c r="L52" s="32" t="s">
         <v>128</v>
@@ -12228,10 +12216,10 @@
         <v>256</v>
       </c>
       <c r="N52" s="32" t="s">
+        <v>494</v>
+      </c>
+      <c r="O52" s="32" t="s">
         <v>495</v>
-      </c>
-      <c r="O52" s="32" t="s">
-        <v>496</v>
       </c>
       <c r="P52" s="33" t="n">
         <v>37104</v>
@@ -12249,16 +12237,16 @@
         <v>98</v>
       </c>
       <c r="U52" s="32" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="V52" s="33" t="n">
         <v>45613</v>
       </c>
       <c r="W52" s="33" t="s">
+        <v>497</v>
+      </c>
+      <c r="X52" s="32" t="s">
         <v>498</v>
-      </c>
-      <c r="X52" s="32" t="s">
-        <v>499</v>
       </c>
       <c r="Y52" s="33" t="n">
         <v>45613</v>
@@ -12267,7 +12255,7 @@
         <v>271</v>
       </c>
       <c r="AA52" s="32" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="AB52" s="33" t="n">
         <v>45614</v>
@@ -12279,31 +12267,31 @@
       <c r="AE52" s="32"/>
       <c r="AF52" s="32"/>
       <c r="AG52" s="32" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="AH52" s="33" t="n">
         <v>45614</v>
       </c>
       <c r="AI52" s="32" t="s">
+        <v>500</v>
+      </c>
+      <c r="AJ52" s="32" t="s">
         <v>501</v>
-      </c>
-      <c r="AJ52" s="32" t="s">
-        <v>502</v>
       </c>
       <c r="AK52" s="33" t="n">
         <v>45660</v>
       </c>
       <c r="AL52" s="32" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="AM52" s="32" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="AN52" s="33" t="n">
         <v>45615</v>
       </c>
       <c r="AO52" s="32" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="AP52" s="32" t="s">
         <v>109</v>
@@ -12379,22 +12367,22 @@
       <c r="H53" s="32"/>
       <c r="I53" s="32"/>
       <c r="J53" s="32" t="s">
+        <v>503</v>
+      </c>
+      <c r="K53" s="32" t="s">
         <v>504</v>
-      </c>
-      <c r="K53" s="32" t="s">
-        <v>505</v>
       </c>
       <c r="L53" s="32" t="s">
         <v>128</v>
       </c>
       <c r="M53" s="32" t="s">
+        <v>505</v>
+      </c>
+      <c r="N53" s="32" t="s">
+        <v>459</v>
+      </c>
+      <c r="O53" s="32" t="s">
         <v>506</v>
-      </c>
-      <c r="N53" s="32" t="s">
-        <v>460</v>
-      </c>
-      <c r="O53" s="32" t="s">
-        <v>507</v>
       </c>
       <c r="P53" s="33" t="n">
         <v>34929</v>
@@ -12412,22 +12400,22 @@
         <v>98</v>
       </c>
       <c r="U53" s="32" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="V53" s="33" t="n">
         <v>45610</v>
       </c>
       <c r="W53" s="33" t="s">
+        <v>507</v>
+      </c>
+      <c r="X53" s="32" t="s">
         <v>508</v>
-      </c>
-      <c r="X53" s="32" t="s">
-        <v>509</v>
       </c>
       <c r="Y53" s="33" t="n">
         <v>45610</v>
       </c>
       <c r="Z53" s="33" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="AA53" s="32"/>
       <c r="AB53" s="33"/>
@@ -12436,7 +12424,7 @@
       <c r="AE53" s="32"/>
       <c r="AF53" s="32"/>
       <c r="AG53" s="32" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="AH53" s="33" t="n">
         <v>45610</v>
@@ -12445,7 +12433,7 @@
         <v>168</v>
       </c>
       <c r="AJ53" s="32" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="AK53" s="33" t="n">
         <v>45661</v>
@@ -12454,13 +12442,13 @@
         <v>168</v>
       </c>
       <c r="AM53" s="32" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="AN53" s="33" t="n">
         <v>45615</v>
       </c>
       <c r="AO53" s="32" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="AP53" s="32" t="s">
         <v>109</v>
@@ -12536,10 +12524,10 @@
       <c r="H54" s="32"/>
       <c r="I54" s="32"/>
       <c r="J54" s="32" t="s">
+        <v>511</v>
+      </c>
+      <c r="K54" s="32" t="s">
         <v>512</v>
-      </c>
-      <c r="K54" s="32" t="s">
-        <v>513</v>
       </c>
       <c r="L54" s="32" t="s">
         <v>128</v>
@@ -12551,7 +12539,7 @@
         <v>331</v>
       </c>
       <c r="O54" s="32" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="P54" s="33" t="n">
         <v>29741</v>
@@ -12569,7 +12557,7 @@
         <v>98</v>
       </c>
       <c r="U54" s="32" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="V54" s="33" t="n">
         <v>45612</v>
@@ -12578,7 +12566,7 @@
         <v>320</v>
       </c>
       <c r="X54" s="32" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="Y54" s="33" t="n">
         <v>45613</v>
@@ -12587,43 +12575,43 @@
         <v>309</v>
       </c>
       <c r="AA54" s="32" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="AB54" s="33" t="n">
         <v>45613</v>
       </c>
       <c r="AC54" s="33" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="AD54" s="32"/>
       <c r="AE54" s="32"/>
       <c r="AF54" s="32"/>
       <c r="AG54" s="32" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="AH54" s="33" t="n">
         <v>45613</v>
       </c>
       <c r="AI54" s="32" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="AJ54" s="32" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="AK54" s="33" t="n">
         <v>45662</v>
       </c>
       <c r="AL54" s="32" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="AM54" s="32" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="AN54" s="33" t="n">
         <v>45615</v>
       </c>
       <c r="AO54" s="32" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="AP54" s="32" t="s">
         <v>109</v>
@@ -12699,10 +12687,10 @@
       <c r="H55" s="32"/>
       <c r="I55" s="32"/>
       <c r="J55" s="32" t="s">
+        <v>519</v>
+      </c>
+      <c r="K55" s="32" t="s">
         <v>520</v>
-      </c>
-      <c r="K55" s="32" t="s">
-        <v>521</v>
       </c>
       <c r="L55" s="32" t="s">
         <v>128</v>
@@ -12711,10 +12699,10 @@
         <v>303</v>
       </c>
       <c r="N55" s="32" t="s">
+        <v>521</v>
+      </c>
+      <c r="O55" s="32" t="s">
         <v>522</v>
-      </c>
-      <c r="O55" s="32" t="s">
-        <v>523</v>
       </c>
       <c r="P55" s="33" t="n">
         <v>31350</v>
@@ -12732,7 +12720,7 @@
         <v>98</v>
       </c>
       <c r="U55" s="32" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="V55" s="33" t="n">
         <v>45612</v>
@@ -12741,7 +12729,7 @@
         <v>320</v>
       </c>
       <c r="X55" s="32" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="Y55" s="33" t="n">
         <v>45613</v>
@@ -12750,43 +12738,43 @@
         <v>309</v>
       </c>
       <c r="AA55" s="32" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="AB55" s="33" t="n">
         <v>45613</v>
       </c>
       <c r="AC55" s="33" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="AD55" s="32"/>
       <c r="AE55" s="32"/>
       <c r="AF55" s="32"/>
       <c r="AG55" s="32" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="AH55" s="33" t="n">
         <v>45613</v>
       </c>
       <c r="AI55" s="32" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="AJ55" s="32" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="AK55" s="33" t="n">
         <v>45663</v>
       </c>
       <c r="AL55" s="32" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="AM55" s="32" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="AN55" s="33" t="n">
         <v>45615</v>
       </c>
       <c r="AO55" s="32" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="AP55" s="32" t="s">
         <v>109</v>
@@ -12862,10 +12850,10 @@
       <c r="H56" s="32"/>
       <c r="I56" s="32"/>
       <c r="J56" s="32" t="s">
+        <v>525</v>
+      </c>
+      <c r="K56" s="32" t="s">
         <v>526</v>
-      </c>
-      <c r="K56" s="32" t="s">
-        <v>527</v>
       </c>
       <c r="L56" s="32" t="s">
         <v>128</v>
@@ -12877,7 +12865,7 @@
         <v>331</v>
       </c>
       <c r="O56" s="32" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="P56" s="33" t="n">
         <v>25535</v>
@@ -12895,7 +12883,7 @@
         <v>98</v>
       </c>
       <c r="U56" s="32" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="V56" s="33" t="n">
         <v>45612</v>
@@ -12904,7 +12892,7 @@
         <v>320</v>
       </c>
       <c r="X56" s="32" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="Y56" s="33" t="n">
         <v>45613</v>
@@ -12913,43 +12901,43 @@
         <v>309</v>
       </c>
       <c r="AA56" s="32" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="AB56" s="33" t="n">
         <v>45613</v>
       </c>
       <c r="AC56" s="33" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="AD56" s="32"/>
       <c r="AE56" s="32"/>
       <c r="AF56" s="32"/>
       <c r="AG56" s="32" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="AH56" s="33" t="n">
         <v>45613</v>
       </c>
       <c r="AI56" s="32" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="AJ56" s="32" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="AK56" s="33" t="n">
         <v>45664</v>
       </c>
       <c r="AL56" s="32" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="AM56" s="32" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="AN56" s="33" t="n">
         <v>45615</v>
       </c>
       <c r="AO56" s="32" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="AP56" s="32" t="s">
         <v>109</v>
@@ -13025,10 +13013,10 @@
       <c r="H57" s="32"/>
       <c r="I57" s="32"/>
       <c r="J57" s="32" t="s">
+        <v>530</v>
+      </c>
+      <c r="K57" s="32" t="s">
         <v>531</v>
-      </c>
-      <c r="K57" s="32" t="s">
-        <v>532</v>
       </c>
       <c r="L57" s="32" t="s">
         <v>128</v>
@@ -13040,7 +13028,7 @@
         <v>344</v>
       </c>
       <c r="O57" s="32" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="P57" s="33" t="n">
         <v>32349</v>
@@ -13058,7 +13046,7 @@
         <v>98</v>
       </c>
       <c r="U57" s="32" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="V57" s="33" t="n">
         <v>45612</v>
@@ -13067,7 +13055,7 @@
         <v>320</v>
       </c>
       <c r="X57" s="32" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="Y57" s="33" t="n">
         <v>45613</v>
@@ -13076,43 +13064,43 @@
         <v>309</v>
       </c>
       <c r="AA57" s="32" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="AB57" s="33" t="n">
         <v>45613</v>
       </c>
       <c r="AC57" s="33" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="AD57" s="32"/>
       <c r="AE57" s="32"/>
       <c r="AF57" s="32"/>
       <c r="AG57" s="32" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="AH57" s="33" t="n">
         <v>45613</v>
       </c>
       <c r="AI57" s="32" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="AJ57" s="32" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="AK57" s="33" t="n">
         <v>45665</v>
       </c>
       <c r="AL57" s="32" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="AM57" s="32" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="AN57" s="33" t="n">
         <v>45615</v>
       </c>
       <c r="AO57" s="32" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="AP57" s="32" t="s">
         <v>109</v>
@@ -13188,10 +13176,10 @@
       <c r="H58" s="32"/>
       <c r="I58" s="32"/>
       <c r="J58" s="32" t="s">
+        <v>535</v>
+      </c>
+      <c r="K58" s="32" t="s">
         <v>536</v>
-      </c>
-      <c r="K58" s="32" t="s">
-        <v>537</v>
       </c>
       <c r="L58" s="32" t="s">
         <v>92</v>
@@ -13203,7 +13191,7 @@
         <v>186</v>
       </c>
       <c r="O58" s="32" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="P58" s="33" t="n">
         <v>28254</v>
@@ -13221,7 +13209,7 @@
         <v>98</v>
       </c>
       <c r="U58" s="32" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="V58" s="33" t="n">
         <v>45612</v>
@@ -13230,7 +13218,7 @@
         <v>320</v>
       </c>
       <c r="X58" s="32" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="Y58" s="33" t="n">
         <v>45613</v>
@@ -13239,43 +13227,43 @@
         <v>309</v>
       </c>
       <c r="AA58" s="32" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="AB58" s="33" t="n">
         <v>45613</v>
       </c>
       <c r="AC58" s="33" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="AD58" s="32"/>
       <c r="AE58" s="32"/>
       <c r="AF58" s="32"/>
       <c r="AG58" s="32" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="AH58" s="33" t="n">
         <v>45613</v>
       </c>
       <c r="AI58" s="32" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="AJ58" s="32" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="AK58" s="33" t="n">
         <v>45666</v>
       </c>
       <c r="AL58" s="32" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="AM58" s="32" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="AN58" s="33" t="n">
         <v>45615</v>
       </c>
       <c r="AO58" s="32" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="AP58" s="32" t="s">
         <v>109</v>
@@ -13351,22 +13339,22 @@
       <c r="H59" s="32"/>
       <c r="I59" s="32"/>
       <c r="J59" s="32" t="s">
+        <v>540</v>
+      </c>
+      <c r="K59" s="32" t="s">
         <v>541</v>
-      </c>
-      <c r="K59" s="32" t="s">
-        <v>542</v>
       </c>
       <c r="L59" s="32" t="s">
         <v>128</v>
       </c>
       <c r="M59" s="32" t="s">
+        <v>542</v>
+      </c>
+      <c r="N59" s="32" t="s">
+        <v>459</v>
+      </c>
+      <c r="O59" s="32" t="s">
         <v>543</v>
-      </c>
-      <c r="N59" s="32" t="s">
-        <v>460</v>
-      </c>
-      <c r="O59" s="32" t="s">
-        <v>544</v>
       </c>
       <c r="P59" s="33" t="n">
         <v>30460</v>
@@ -13384,37 +13372,37 @@
         <v>98</v>
       </c>
       <c r="U59" s="32" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="V59" s="33" t="n">
         <v>45608</v>
       </c>
       <c r="W59" s="33" t="s">
+        <v>544</v>
+      </c>
+      <c r="X59" s="32" t="s">
         <v>545</v>
-      </c>
-      <c r="X59" s="32" t="s">
-        <v>546</v>
       </c>
       <c r="Y59" s="33" t="n">
         <v>45609</v>
       </c>
       <c r="Z59" s="33" t="s">
+        <v>546</v>
+      </c>
+      <c r="AA59" s="32" t="s">
         <v>547</v>
-      </c>
-      <c r="AA59" s="32" t="s">
-        <v>548</v>
       </c>
       <c r="AB59" s="33" t="n">
         <v>45609</v>
       </c>
       <c r="AC59" s="33" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="AD59" s="32"/>
       <c r="AE59" s="32"/>
       <c r="AF59" s="32"/>
       <c r="AG59" s="32" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="AH59" s="33" t="n">
         <v>45609</v>
@@ -13423,7 +13411,7 @@
         <v>168</v>
       </c>
       <c r="AJ59" s="32" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="AK59" s="33" t="n">
         <v>45667</v>
@@ -13432,13 +13420,13 @@
         <v>168</v>
       </c>
       <c r="AM59" s="32" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="AN59" s="33" t="n">
         <v>45615</v>
       </c>
       <c r="AO59" s="32" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="AP59" s="32" t="s">
         <v>109</v>
@@ -13514,22 +13502,22 @@
       <c r="H60" s="32"/>
       <c r="I60" s="32"/>
       <c r="J60" s="32" t="s">
+        <v>550</v>
+      </c>
+      <c r="K60" s="32" t="s">
         <v>551</v>
-      </c>
-      <c r="K60" s="32" t="s">
-        <v>552</v>
       </c>
       <c r="L60" s="32" t="s">
         <v>92</v>
       </c>
       <c r="M60" s="32" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="N60" s="32" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="O60" s="32" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="P60" s="33" t="n">
         <v>34043</v>
@@ -13547,7 +13535,7 @@
         <v>98</v>
       </c>
       <c r="U60" s="32" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="V60" s="33" t="n">
         <v>45613</v>
@@ -13556,13 +13544,13 @@
         <v>148</v>
       </c>
       <c r="X60" s="32" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="Y60" s="33" t="n">
         <v>45613</v>
       </c>
       <c r="Z60" s="33" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="AA60" s="32"/>
       <c r="AB60" s="33"/>
@@ -13571,7 +13559,7 @@
       <c r="AE60" s="32"/>
       <c r="AF60" s="32"/>
       <c r="AG60" s="32" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="AH60" s="33" t="n">
         <v>45613</v>
@@ -13580,7 +13568,7 @@
         <v>221</v>
       </c>
       <c r="AJ60" s="32" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="AK60" s="33" t="n">
         <v>45668</v>
@@ -13589,13 +13577,13 @@
         <v>221</v>
       </c>
       <c r="AM60" s="32" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="AN60" s="33" t="n">
         <v>45615</v>
       </c>
       <c r="AO60" s="32" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="AP60" s="32" t="s">
         <v>109</v>
@@ -13671,22 +13659,22 @@
       <c r="H61" s="32"/>
       <c r="I61" s="32"/>
       <c r="J61" s="32" t="s">
+        <v>555</v>
+      </c>
+      <c r="K61" s="32" t="s">
         <v>556</v>
-      </c>
-      <c r="K61" s="32" t="s">
-        <v>557</v>
       </c>
       <c r="L61" s="32" t="s">
         <v>128</v>
       </c>
       <c r="M61" s="32" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="N61" s="32" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="O61" s="32" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="P61" s="33" t="n">
         <v>34862</v>
@@ -13704,7 +13692,7 @@
         <v>98</v>
       </c>
       <c r="U61" s="32" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="V61" s="33" t="n">
         <v>45613</v>
@@ -13713,7 +13701,7 @@
         <v>148</v>
       </c>
       <c r="X61" s="32" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="Y61" s="33" t="n">
         <v>45614</v>
@@ -13728,7 +13716,7 @@
       <c r="AE61" s="32"/>
       <c r="AF61" s="32"/>
       <c r="AG61" s="32" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="AH61" s="33" t="n">
         <v>45614</v>
@@ -13737,7 +13725,7 @@
         <v>252</v>
       </c>
       <c r="AJ61" s="32" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="AK61" s="33" t="n">
         <v>45669</v>
@@ -13746,13 +13734,13 @@
         <v>252</v>
       </c>
       <c r="AM61" s="32" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="AN61" s="33" t="n">
         <v>45615</v>
       </c>
       <c r="AO61" s="32" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="AP61" s="32" t="s">
         <v>109</v>
@@ -13828,10 +13816,10 @@
       <c r="H62" s="32"/>
       <c r="I62" s="32"/>
       <c r="J62" s="32" t="s">
+        <v>559</v>
+      </c>
+      <c r="K62" s="32" t="s">
         <v>560</v>
-      </c>
-      <c r="K62" s="32" t="s">
-        <v>561</v>
       </c>
       <c r="L62" s="32" t="s">
         <v>128</v>
@@ -13843,7 +13831,7 @@
         <v>219</v>
       </c>
       <c r="O62" s="32" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="P62" s="33" t="n">
         <v>29744</v>
@@ -13861,16 +13849,16 @@
         <v>98</v>
       </c>
       <c r="U62" s="32" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="V62" s="33" t="n">
         <v>45613</v>
       </c>
       <c r="W62" s="33" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="X62" s="32" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="Y62" s="33" t="n">
         <v>45613</v>
@@ -13879,19 +13867,19 @@
         <v>102</v>
       </c>
       <c r="AA62" s="32" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="AB62" s="33" t="n">
         <v>45613</v>
       </c>
       <c r="AC62" s="33" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="AD62" s="32"/>
       <c r="AE62" s="32"/>
       <c r="AF62" s="32"/>
       <c r="AG62" s="32" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="AH62" s="33" t="n">
         <v>45613</v>
@@ -13900,7 +13888,7 @@
         <v>299</v>
       </c>
       <c r="AJ62" s="32" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="AK62" s="33" t="n">
         <v>45670</v>
@@ -13909,13 +13897,13 @@
         <v>299</v>
       </c>
       <c r="AM62" s="32" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="AN62" s="33" t="n">
         <v>45615</v>
       </c>
       <c r="AO62" s="32" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="AP62" s="32" t="s">
         <v>109</v>
@@ -13991,22 +13979,22 @@
       <c r="H63" s="32"/>
       <c r="I63" s="32"/>
       <c r="J63" s="32" t="s">
+        <v>564</v>
+      </c>
+      <c r="K63" s="32" t="s">
         <v>565</v>
-      </c>
-      <c r="K63" s="32" t="s">
-        <v>566</v>
       </c>
       <c r="L63" s="32" t="s">
         <v>92</v>
       </c>
       <c r="M63" s="32" t="s">
+        <v>566</v>
+      </c>
+      <c r="N63" s="32" t="s">
+        <v>459</v>
+      </c>
+      <c r="O63" s="32" t="s">
         <v>567</v>
-      </c>
-      <c r="N63" s="32" t="s">
-        <v>460</v>
-      </c>
-      <c r="O63" s="32" t="s">
-        <v>568</v>
       </c>
       <c r="P63" s="33" t="n">
         <v>26701</v>
@@ -14024,13 +14012,13 @@
         <v>98</v>
       </c>
       <c r="U63" s="32" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="V63" s="33" t="n">
         <v>45609</v>
       </c>
       <c r="W63" s="33" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="X63" s="32" t="s">
         <v>310</v>
@@ -14039,7 +14027,7 @@
         <v>45609</v>
       </c>
       <c r="Z63" s="33" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="AA63" s="32"/>
       <c r="AB63" s="33"/>
@@ -14048,7 +14036,7 @@
       <c r="AE63" s="32"/>
       <c r="AF63" s="32"/>
       <c r="AG63" s="32" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="AH63" s="33" t="n">
         <v>45609</v>
@@ -14057,7 +14045,7 @@
         <v>340</v>
       </c>
       <c r="AJ63" s="32" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="AK63" s="33" t="n">
         <v>45671</v>
@@ -14066,13 +14054,13 @@
         <v>340</v>
       </c>
       <c r="AM63" s="32" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="AN63" s="33" t="n">
         <v>45615</v>
       </c>
       <c r="AO63" s="32" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="AP63" s="32" t="s">
         <v>109</v>
@@ -14148,31 +14136,31 @@
       <c r="H64" s="32"/>
       <c r="I64" s="32"/>
       <c r="J64" s="32" t="s">
+        <v>570</v>
+      </c>
+      <c r="K64" s="32" t="s">
         <v>571</v>
-      </c>
-      <c r="K64" s="32" t="s">
-        <v>572</v>
       </c>
       <c r="L64" s="32" t="s">
         <v>128</v>
       </c>
       <c r="M64" s="32" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="N64" s="32" t="s">
         <v>142</v>
       </c>
       <c r="O64" s="32" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="P64" s="33" t="n">
         <v>24200</v>
       </c>
       <c r="Q64" s="32" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="R64" s="32" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="S64" s="32" t="s">
         <v>98</v>
@@ -14181,22 +14169,22 @@
         <v>98</v>
       </c>
       <c r="U64" s="32" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="V64" s="33" t="n">
         <v>45613</v>
       </c>
       <c r="W64" s="33" t="s">
+        <v>575</v>
+      </c>
+      <c r="X64" s="32" t="s">
         <v>576</v>
-      </c>
-      <c r="X64" s="32" t="s">
-        <v>577</v>
       </c>
       <c r="Y64" s="33" t="n">
         <v>45613</v>
       </c>
       <c r="Z64" s="33" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="AA64" s="32"/>
       <c r="AB64" s="33"/>
@@ -14205,7 +14193,7 @@
       <c r="AE64" s="32"/>
       <c r="AF64" s="32"/>
       <c r="AG64" s="32" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="AH64" s="33" t="n">
         <v>45613</v>
@@ -14214,7 +14202,7 @@
         <v>369</v>
       </c>
       <c r="AJ64" s="32" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="AK64" s="33" t="n">
         <v>45672</v>
@@ -14223,13 +14211,13 @@
         <v>369</v>
       </c>
       <c r="AM64" s="32" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="AN64" s="33" t="n">
         <v>45615</v>
       </c>
       <c r="AO64" s="32" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="AP64" s="32" t="s">
         <v>109</v>
@@ -14305,70 +14293,70 @@
       <c r="H65" s="32"/>
       <c r="I65" s="32"/>
       <c r="J65" s="32" t="s">
+        <v>578</v>
+      </c>
+      <c r="K65" s="32" t="s">
         <v>579</v>
-      </c>
-      <c r="K65" s="32" t="s">
-        <v>580</v>
       </c>
       <c r="L65" s="32" t="s">
         <v>128</v>
       </c>
       <c r="M65" s="32" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="N65" s="32" t="s">
+        <v>580</v>
+      </c>
+      <c r="O65" s="32" t="s">
         <v>581</v>
-      </c>
-      <c r="O65" s="32" t="s">
-        <v>582</v>
       </c>
       <c r="P65" s="33" t="n">
         <v>29879</v>
       </c>
       <c r="Q65" s="32" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="R65" s="32" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="S65" s="32" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="T65" s="32" t="s">
         <v>98</v>
       </c>
       <c r="U65" s="32" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="V65" s="33" t="n">
         <v>45613</v>
       </c>
       <c r="W65" s="33" t="s">
+        <v>583</v>
+      </c>
+      <c r="X65" s="32" t="s">
         <v>584</v>
-      </c>
-      <c r="X65" s="32" t="s">
-        <v>585</v>
       </c>
       <c r="Y65" s="33" t="n">
         <v>45613</v>
       </c>
       <c r="Z65" s="33" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="AA65" s="32" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="AB65" s="33" t="n">
         <v>45613</v>
       </c>
       <c r="AC65" s="33" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="AD65" s="32"/>
       <c r="AE65" s="32"/>
       <c r="AF65" s="32"/>
       <c r="AG65" s="32" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="AH65" s="33" t="n">
         <v>45613</v>
@@ -14377,7 +14365,7 @@
         <v>396</v>
       </c>
       <c r="AJ65" s="32" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="AK65" s="33" t="n">
         <v>45673</v>
@@ -14386,13 +14374,13 @@
         <v>396</v>
       </c>
       <c r="AM65" s="32" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="AN65" s="33" t="n">
         <v>45615</v>
       </c>
       <c r="AO65" s="32" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="AP65" s="32" t="s">
         <v>109</v>
@@ -14468,28 +14456,28 @@
       <c r="H66" s="32"/>
       <c r="I66" s="32"/>
       <c r="J66" s="32" t="s">
+        <v>587</v>
+      </c>
+      <c r="K66" s="32" t="s">
         <v>588</v>
-      </c>
-      <c r="K66" s="32" t="s">
-        <v>589</v>
       </c>
       <c r="L66" s="32" t="s">
         <v>128</v>
       </c>
       <c r="M66" s="32" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="N66" s="32" t="s">
+        <v>589</v>
+      </c>
+      <c r="O66" s="32" t="s">
         <v>590</v>
-      </c>
-      <c r="O66" s="32" t="s">
-        <v>591</v>
       </c>
       <c r="P66" s="33" t="n">
         <v>28476</v>
       </c>
       <c r="Q66" s="32" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="R66" s="32" t="s">
         <v>97</v>
@@ -14501,37 +14489,37 @@
         <v>98</v>
       </c>
       <c r="U66" s="32" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="V66" s="33" t="n">
         <v>45613</v>
       </c>
       <c r="W66" s="33" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="X66" s="32" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="Y66" s="33" t="n">
         <v>45613</v>
       </c>
       <c r="Z66" s="33" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="AA66" s="32" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="AB66" s="33" t="n">
         <v>45614</v>
       </c>
       <c r="AC66" s="33" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="AD66" s="32"/>
       <c r="AE66" s="32"/>
       <c r="AF66" s="32"/>
       <c r="AG66" s="32" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="AH66" s="33" t="n">
         <v>45614</v>
@@ -14540,7 +14528,7 @@
         <v>401</v>
       </c>
       <c r="AJ66" s="32" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="AK66" s="33" t="n">
         <v>45674</v>
@@ -14549,13 +14537,13 @@
         <v>401</v>
       </c>
       <c r="AM66" s="32" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="AN66" s="33" t="n">
         <v>45615</v>
       </c>
       <c r="AO66" s="32" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="AP66" s="32" t="s">
         <v>109</v>
@@ -14631,22 +14619,22 @@
       <c r="H67" s="32"/>
       <c r="I67" s="32"/>
       <c r="J67" s="32" t="s">
+        <v>595</v>
+      </c>
+      <c r="K67" s="32" t="s">
         <v>596</v>
-      </c>
-      <c r="K67" s="32" t="s">
-        <v>597</v>
       </c>
       <c r="L67" s="32" t="s">
         <v>92</v>
       </c>
       <c r="M67" s="32" t="s">
+        <v>597</v>
+      </c>
+      <c r="N67" s="32" t="s">
         <v>598</v>
       </c>
-      <c r="N67" s="32" t="s">
+      <c r="O67" s="32" t="s">
         <v>599</v>
-      </c>
-      <c r="O67" s="32" t="s">
-        <v>600</v>
       </c>
       <c r="P67" s="33" t="n">
         <v>28646</v>
@@ -14664,22 +14652,22 @@
         <v>98</v>
       </c>
       <c r="U67" s="32" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="V67" s="33" t="n">
         <v>45613</v>
       </c>
       <c r="W67" s="33" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="X67" s="32" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="Y67" s="33" t="n">
         <v>45614</v>
       </c>
       <c r="Z67" s="33" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="AA67" s="32"/>
       <c r="AB67" s="33"/>
@@ -14688,7 +14676,7 @@
       <c r="AE67" s="32"/>
       <c r="AF67" s="32"/>
       <c r="AG67" s="32" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="AH67" s="33" t="n">
         <v>45614</v>
@@ -14697,7 +14685,7 @@
         <v>409</v>
       </c>
       <c r="AJ67" s="32" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="AK67" s="33" t="n">
         <v>45675</v>
@@ -14706,13 +14694,13 @@
         <v>409</v>
       </c>
       <c r="AM67" s="32" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="AN67" s="33" t="n">
         <v>45615</v>
       </c>
       <c r="AO67" s="32" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="AP67" s="32" t="s">
         <v>109</v>
@@ -14788,31 +14776,31 @@
       <c r="H68" s="32"/>
       <c r="I68" s="32"/>
       <c r="J68" s="32" t="s">
+        <v>603</v>
+      </c>
+      <c r="K68" s="32" t="s">
         <v>604</v>
-      </c>
-      <c r="K68" s="32" t="s">
-        <v>605</v>
       </c>
       <c r="L68" s="32" t="s">
         <v>92</v>
       </c>
       <c r="M68" s="32" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="N68" s="32" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="O68" s="32" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="P68" s="33" t="n">
         <v>34573</v>
       </c>
       <c r="Q68" s="32" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="R68" s="32" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="S68" s="32" t="s">
         <v>98</v>
@@ -14821,22 +14809,22 @@
         <v>98</v>
       </c>
       <c r="U68" s="32" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="V68" s="33" t="n">
         <v>45609</v>
       </c>
       <c r="W68" s="33" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="X68" s="32" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="Y68" s="33" t="n">
         <v>45609</v>
       </c>
       <c r="Z68" s="33" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="AA68" s="32"/>
       <c r="AB68" s="33"/>
@@ -14845,31 +14833,31 @@
       <c r="AE68" s="32"/>
       <c r="AF68" s="32"/>
       <c r="AG68" s="32" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="AH68" s="33" t="n">
         <v>45609</v>
       </c>
       <c r="AI68" s="32" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="AJ68" s="32" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="AK68" s="33" t="n">
         <v>45676</v>
       </c>
       <c r="AL68" s="32" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="AM68" s="32" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="AN68" s="33" t="n">
         <v>45615</v>
       </c>
       <c r="AO68" s="32" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="AP68" s="32" t="s">
         <v>109</v>
@@ -14945,28 +14933,28 @@
       <c r="H69" s="32"/>
       <c r="I69" s="32"/>
       <c r="J69" s="32" t="s">
+        <v>609</v>
+      </c>
+      <c r="K69" s="32" t="s">
         <v>610</v>
-      </c>
-      <c r="K69" s="32" t="s">
-        <v>611</v>
       </c>
       <c r="L69" s="32" t="s">
         <v>128</v>
       </c>
       <c r="M69" s="32" t="s">
+        <v>611</v>
+      </c>
+      <c r="N69" s="32" t="s">
+        <v>459</v>
+      </c>
+      <c r="O69" s="32" t="s">
         <v>612</v>
-      </c>
-      <c r="N69" s="32" t="s">
-        <v>460</v>
-      </c>
-      <c r="O69" s="32" t="s">
-        <v>613</v>
       </c>
       <c r="P69" s="33" t="n">
         <v>29004</v>
       </c>
       <c r="Q69" s="32" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="R69" s="32" t="s">
         <v>96</v>
@@ -14978,67 +14966,67 @@
         <v>97</v>
       </c>
       <c r="U69" s="32" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="V69" s="33" t="n">
         <v>45608</v>
       </c>
       <c r="W69" s="33" t="s">
+        <v>614</v>
+      </c>
+      <c r="X69" s="32" t="s">
         <v>615</v>
-      </c>
-      <c r="X69" s="32" t="s">
-        <v>616</v>
       </c>
       <c r="Y69" s="33" t="n">
         <v>45608</v>
       </c>
       <c r="Z69" s="33" t="s">
+        <v>616</v>
+      </c>
+      <c r="AA69" s="32" t="s">
         <v>617</v>
-      </c>
-      <c r="AA69" s="32" t="s">
-        <v>618</v>
       </c>
       <c r="AB69" s="33" t="n">
         <v>45609</v>
       </c>
       <c r="AC69" s="33" t="s">
+        <v>618</v>
+      </c>
+      <c r="AD69" s="32" t="s">
         <v>619</v>
-      </c>
-      <c r="AD69" s="32" t="s">
-        <v>620</v>
       </c>
       <c r="AE69" s="33" t="n">
         <v>45609</v>
       </c>
       <c r="AF69" s="32" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="AG69" s="32" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="AH69" s="33" t="n">
         <v>45609</v>
       </c>
       <c r="AI69" s="32" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="AJ69" s="32" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="AK69" s="33" t="n">
         <v>45677</v>
       </c>
       <c r="AL69" s="32" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="AM69" s="32" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="AN69" s="33" t="n">
         <v>45615</v>
       </c>
       <c r="AO69" s="32" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="AP69" s="32" t="s">
         <v>109</v>
@@ -15631,8 +15619,8 @@
   </sheetPr>
   <dimension ref="A1:BV5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="S1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="W5" activeCellId="0" sqref="W5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15718,7 +15706,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="28" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="D1" s="28" t="s">
         <v>3</v>
@@ -15727,13 +15715,13 @@
         <v>4</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="G1" s="10" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="I1" s="12" t="s">
         <v>8</v>
@@ -15957,28 +15945,28 @@
         <v>125</v>
       </c>
       <c r="H2" s="32" t="s">
+        <v>626</v>
+      </c>
+      <c r="I2" s="32" t="s">
+        <v>626</v>
+      </c>
+      <c r="J2" s="32" t="s">
         <v>627</v>
       </c>
-      <c r="I2" s="32" t="s">
-        <v>627</v>
-      </c>
-      <c r="J2" s="32" t="s">
+      <c r="K2" s="32" t="s">
         <v>628</v>
-      </c>
-      <c r="K2" s="32" t="s">
-        <v>629</v>
       </c>
       <c r="L2" s="32" t="s">
         <v>128</v>
       </c>
       <c r="M2" s="32" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="N2" s="32" t="s">
         <v>142</v>
       </c>
       <c r="O2" s="32" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="P2" s="33" t="n">
         <v>36506</v>
@@ -15988,13 +15976,13 @@
       <c r="S2" s="32"/>
       <c r="T2" s="32"/>
       <c r="U2" s="32" t="s">
+        <v>631</v>
+      </c>
+      <c r="V2" s="32" t="s">
         <v>632</v>
       </c>
-      <c r="V2" s="32" t="s">
+      <c r="W2" s="32" t="s">
         <v>633</v>
-      </c>
-      <c r="W2" s="32" t="s">
-        <v>634</v>
       </c>
       <c r="X2" s="32"/>
       <c r="Y2" s="32"/>
@@ -16050,10 +16038,10 @@
     </row>
     <row r="3" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="32" t="s">
+        <v>634</v>
+      </c>
+      <c r="B3" s="32" t="s">
         <v>635</v>
-      </c>
-      <c r="B3" s="32" t="s">
-        <v>636</v>
       </c>
       <c r="C3" s="33" t="n">
         <v>45569</v>
@@ -16071,64 +16059,64 @@
         <v>89</v>
       </c>
       <c r="H3" s="32" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="I3" s="32" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J3" s="32" t="s">
+        <v>636</v>
+      </c>
+      <c r="K3" s="32" t="s">
         <v>637</v>
-      </c>
-      <c r="K3" s="32" t="s">
-        <v>638</v>
       </c>
       <c r="L3" s="32" t="s">
         <v>128</v>
       </c>
       <c r="M3" s="32" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="N3" s="32" t="s">
         <v>142</v>
       </c>
       <c r="O3" s="32" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="P3" s="33" t="n">
         <v>24829</v>
       </c>
       <c r="Q3" s="32" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="R3" s="32"/>
       <c r="S3" s="32"/>
       <c r="T3" s="32"/>
       <c r="U3" s="32" t="s">
-        <v>641</v>
-      </c>
-      <c r="V3" s="49" t="n">
-        <v>45557</v>
+        <v>107</v>
+      </c>
+      <c r="V3" s="33" t="n">
+        <v>45611</v>
       </c>
       <c r="W3" s="32" t="s">
-        <v>642</v>
+        <v>108</v>
       </c>
       <c r="X3" s="32" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="Y3" s="33" t="n">
         <v>45557</v>
       </c>
       <c r="Z3" s="32" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="AA3" s="32" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="AB3" s="49" t="n">
         <v>45557</v>
       </c>
       <c r="AC3" s="32" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="AD3" s="32" t="s">
         <v>109</v>
@@ -16143,7 +16131,7 @@
         <v>2</v>
       </c>
       <c r="AH3" s="32" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="AI3" s="49" t="n">
         <v>45557</v>
@@ -16152,13 +16140,13 @@
         <v>45558</v>
       </c>
       <c r="AK3" s="32" t="s">
+        <v>645</v>
+      </c>
+      <c r="AL3" s="32" t="s">
         <v>646</v>
       </c>
-      <c r="AL3" s="32" t="s">
+      <c r="AM3" s="32" t="s">
         <v>647</v>
-      </c>
-      <c r="AM3" s="32" t="s">
-        <v>648</v>
       </c>
       <c r="AN3" s="49" t="n">
         <v>45557</v>
@@ -16167,10 +16155,10 @@
         <v>45558</v>
       </c>
       <c r="AP3" s="32" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="AQ3" s="32" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="AR3" s="32" t="s">
         <v>115</v>
@@ -16182,10 +16170,10 @@
         <v>45558</v>
       </c>
       <c r="AU3" s="32" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="AV3" s="32" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="AW3" s="32" t="s">
         <v>117</v>
@@ -16224,7 +16212,7 @@
         <v>45557</v>
       </c>
       <c r="BI3" s="32" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="BJ3" s="32" t="s">
         <v>263</v>
@@ -16236,7 +16224,7 @@
         <v>45557</v>
       </c>
       <c r="BM3" s="32" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="BN3" s="32" t="s">
         <v>263</v>
@@ -16248,16 +16236,16 @@
         <v>45557</v>
       </c>
       <c r="BQ3" s="32" t="s">
+        <v>650</v>
+      </c>
+      <c r="BR3" s="32" t="s">
         <v>651</v>
-      </c>
-      <c r="BR3" s="32" t="s">
-        <v>652</v>
       </c>
       <c r="BS3" s="32" t="s">
         <v>122</v>
       </c>
       <c r="BT3" s="32" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="BU3" s="49" t="n">
         <v>45557</v>
@@ -16268,10 +16256,10 @@
     </row>
     <row r="4" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="32" t="s">
+        <v>653</v>
+      </c>
+      <c r="B4" s="32" t="s">
         <v>654</v>
-      </c>
-      <c r="B4" s="32" t="s">
-        <v>655</v>
       </c>
       <c r="C4" s="33" t="n">
         <v>45918</v>
@@ -16283,55 +16271,55 @@
         <v>45918</v>
       </c>
       <c r="F4" s="32" t="s">
+        <v>655</v>
+      </c>
+      <c r="G4" s="32" t="s">
         <v>656</v>
-      </c>
-      <c r="G4" s="32" t="s">
-        <v>657</v>
       </c>
       <c r="H4" s="32"/>
       <c r="I4" s="32"/>
       <c r="J4" s="32" t="s">
+        <v>657</v>
+      </c>
+      <c r="K4" s="32" t="s">
         <v>658</v>
-      </c>
-      <c r="K4" s="32" t="s">
-        <v>659</v>
       </c>
       <c r="L4" s="32" t="s">
         <v>92</v>
       </c>
       <c r="M4" s="32" t="s">
+        <v>659</v>
+      </c>
+      <c r="N4" s="32" t="s">
         <v>660</v>
       </c>
-      <c r="N4" s="32" t="s">
+      <c r="O4" s="32" t="s">
         <v>661</v>
       </c>
-      <c r="O4" s="32" t="s">
+      <c r="P4" s="33" t="s">
         <v>662</v>
-      </c>
-      <c r="P4" s="33" t="s">
-        <v>663</v>
       </c>
       <c r="Q4" s="32"/>
       <c r="R4" s="32"/>
       <c r="S4" s="32"/>
       <c r="T4" s="32"/>
       <c r="U4" s="32" t="s">
-        <v>664</v>
-      </c>
-      <c r="V4" s="49" t="n">
-        <v>45558</v>
+        <v>107</v>
+      </c>
+      <c r="V4" s="33" t="n">
+        <v>45611</v>
       </c>
       <c r="W4" s="32" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="X4" s="32" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="Y4" s="33" t="n">
         <v>45558</v>
       </c>
       <c r="Z4" s="32" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="AA4" s="32"/>
       <c r="AB4" s="32"/>
@@ -16381,7 +16369,7 @@
       <c r="BR4" s="32"/>
       <c r="BS4" s="32"/>
       <c r="BT4" s="32" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="BU4" s="32"/>
       <c r="BV4" s="32" t="s">

</xml_diff>

<commit_message>
Asignación de vuelos on y off
</commit_message>
<xml_diff>
--- a/ejemplo_carga_masiva.xlsx
+++ b/ejemplo_carga_masiva.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2425" uniqueCount="620">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2425" uniqueCount="600">
   <si>
     <t xml:space="preserve">Owner</t>
   </si>
@@ -1292,7 +1292,7 @@
     <t xml:space="preserve">CHARTERDAP PUQ-WPU</t>
   </si>
   <si>
-    <t xml:space="preserve">10:00-12:36</t>
+    <t xml:space="preserve">10:00-12:57</t>
   </si>
   <si>
     <t xml:space="preserve">NAULAK</t>
@@ -1307,9 +1307,6 @@
     <t xml:space="preserve">R8779096</t>
   </si>
   <si>
-    <t xml:space="preserve">10:00-12:37</t>
-  </si>
-  <si>
     <t xml:space="preserve">ARKANI</t>
   </si>
   <si>
@@ -1343,9 +1340,6 @@
     <t xml:space="preserve"> 04:33-7:57</t>
   </si>
   <si>
-    <t xml:space="preserve">10:00-12:38</t>
-  </si>
-  <si>
     <t xml:space="preserve">PERMANA</t>
   </si>
   <si>
@@ -1364,9 +1358,6 @@
     <t xml:space="preserve"> 19:53-23:19</t>
   </si>
   <si>
-    <t xml:space="preserve">10:00-12:39</t>
-  </si>
-  <si>
     <t xml:space="preserve">BARNABA</t>
   </si>
   <si>
@@ -1397,9 +1388,6 @@
     <t xml:space="preserve"> 11:17-14:44</t>
   </si>
   <si>
-    <t xml:space="preserve">10:00-12:40</t>
-  </si>
-  <si>
     <t xml:space="preserve">GRANT</t>
   </si>
   <si>
@@ -1421,9 +1409,6 @@
     <t xml:space="preserve">19:05-14:10+1</t>
   </si>
   <si>
-    <t xml:space="preserve">10:00-12:41</t>
-  </si>
-  <si>
     <t xml:space="preserve">ALDAY</t>
   </si>
   <si>
@@ -1445,9 +1430,6 @@
     <t xml:space="preserve"> 16:31-21:20</t>
   </si>
   <si>
-    <t xml:space="preserve">10:00-12:42</t>
-  </si>
-  <si>
     <t xml:space="preserve">DELA CRUZ</t>
   </si>
   <si>
@@ -1463,9 +1445,6 @@
     <t xml:space="preserve"> 16:31-21:21</t>
   </si>
   <si>
-    <t xml:space="preserve">10:00-12:43</t>
-  </si>
-  <si>
     <t xml:space="preserve">FELISILDA</t>
   </si>
   <si>
@@ -1478,9 +1457,6 @@
     <t xml:space="preserve"> 16:31-21:22</t>
   </si>
   <si>
-    <t xml:space="preserve">10:00-12:44</t>
-  </si>
-  <si>
     <t xml:space="preserve">ISIDORO</t>
   </si>
   <si>
@@ -1505,9 +1481,6 @@
     <t xml:space="preserve">P4521949B</t>
   </si>
   <si>
-    <t xml:space="preserve">10:00-12:46+1</t>
-  </si>
-  <si>
     <t xml:space="preserve">BREDENKAMP</t>
   </si>
   <si>
@@ -1535,9 +1508,6 @@
     <t xml:space="preserve">18:30-07:00+1</t>
   </si>
   <si>
-    <t xml:space="preserve">10:00-12:47</t>
-  </si>
-  <si>
     <t xml:space="preserve">OOSTHUYSE</t>
   </si>
   <si>
@@ -1550,9 +1520,6 @@
     <t xml:space="preserve">23:50-04:15+1</t>
   </si>
   <si>
-    <t xml:space="preserve">10:00-12:48</t>
-  </si>
-  <si>
     <t xml:space="preserve">THORP</t>
   </si>
   <si>
@@ -1562,9 +1529,6 @@
     <t xml:space="preserve">A10073471</t>
   </si>
   <si>
-    <t xml:space="preserve">10:00-12:49</t>
-  </si>
-  <si>
     <t xml:space="preserve">KUMARA</t>
   </si>
   <si>
@@ -1577,9 +1541,6 @@
     <t xml:space="preserve">03:25-06:00</t>
   </si>
   <si>
-    <t xml:space="preserve">10:00-12:50</t>
-  </si>
-  <si>
     <t xml:space="preserve">LUNDSTROEM</t>
   </si>
   <si>
@@ -1598,9 +1559,6 @@
     <t xml:space="preserve"> 19:46-23:22</t>
   </si>
   <si>
-    <t xml:space="preserve">10:00-12:51</t>
-  </si>
-  <si>
     <t xml:space="preserve">DOMANIN</t>
   </si>
   <si>
@@ -1622,9 +1580,6 @@
     <t xml:space="preserve">KL701 AMS-SCL</t>
   </si>
   <si>
-    <t xml:space="preserve">10:00-12:52</t>
-  </si>
-  <si>
     <t xml:space="preserve">MURTAKOV</t>
   </si>
   <si>
@@ -1649,9 +1604,6 @@
     <t xml:space="preserve">17:25-19:25</t>
   </si>
   <si>
-    <t xml:space="preserve">10:00-12:53+1</t>
-  </si>
-  <si>
     <t xml:space="preserve">SULZHUK</t>
   </si>
   <si>
@@ -1673,9 +1625,6 @@
     <t xml:space="preserve">07:15-11:25</t>
   </si>
   <si>
-    <t xml:space="preserve">10:00-12:54</t>
-  </si>
-  <si>
     <t xml:space="preserve">ALLAN</t>
   </si>
   <si>
@@ -1697,9 +1646,6 @@
     <t xml:space="preserve">08:35-13:00</t>
   </si>
   <si>
-    <t xml:space="preserve">10:00-12:55</t>
-  </si>
-  <si>
     <t xml:space="preserve">MELLUISH</t>
   </si>
   <si>
@@ -1712,9 +1658,6 @@
     <t xml:space="preserve">17:05-19:25</t>
   </si>
   <si>
-    <t xml:space="preserve">10:00-12:56</t>
-  </si>
-  <si>
     <t xml:space="preserve">KWIDINI</t>
   </si>
   <si>
@@ -1749,9 +1692,6 @@
   </si>
   <si>
     <t xml:space="preserve"> 23:35-09:20+1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10:00-12:57</t>
   </si>
   <si>
     <t xml:space="preserve">Date First Flight</t>
@@ -2443,8 +2383,8 @@
   </sheetPr>
   <dimension ref="A1:CH75"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AG1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AK38" activeCellId="0" sqref="AK38"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AG46" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AO48" activeCellId="0" sqref="AO48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11681,7 +11621,7 @@
         <v>45615</v>
       </c>
       <c r="AO49" s="32" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="AP49" s="32" t="s">
         <v>109</v>
@@ -11757,10 +11697,10 @@
       <c r="H50" s="32"/>
       <c r="I50" s="32"/>
       <c r="J50" s="32" t="s">
+        <v>428</v>
+      </c>
+      <c r="K50" s="32" t="s">
         <v>429</v>
-      </c>
-      <c r="K50" s="32" t="s">
-        <v>430</v>
       </c>
       <c r="L50" s="32" t="s">
         <v>128</v>
@@ -11769,10 +11709,10 @@
         <v>233</v>
       </c>
       <c r="N50" s="32" t="s">
+        <v>430</v>
+      </c>
+      <c r="O50" s="32" t="s">
         <v>431</v>
-      </c>
-      <c r="O50" s="32" t="s">
-        <v>432</v>
       </c>
       <c r="P50" s="33" t="n">
         <v>34162</v>
@@ -11790,16 +11730,16 @@
         <v>98</v>
       </c>
       <c r="U50" s="32" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="V50" s="33" t="n">
         <v>45613</v>
       </c>
       <c r="W50" s="33" t="s">
+        <v>433</v>
+      </c>
+      <c r="X50" s="32" t="s">
         <v>434</v>
-      </c>
-      <c r="X50" s="32" t="s">
-        <v>435</v>
       </c>
       <c r="Y50" s="33" t="n">
         <v>45613</v>
@@ -11808,34 +11748,34 @@
         <v>102</v>
       </c>
       <c r="AA50" s="32" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="AB50" s="33" t="n">
         <v>45613</v>
       </c>
       <c r="AC50" s="33" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="AD50" s="32"/>
       <c r="AE50" s="32"/>
       <c r="AF50" s="32"/>
       <c r="AG50" s="32" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="AH50" s="33" t="n">
         <v>45613</v>
       </c>
       <c r="AI50" s="33" t="s">
+        <v>436</v>
+      </c>
+      <c r="AJ50" s="32" t="s">
         <v>437</v>
-      </c>
-      <c r="AJ50" s="32" t="s">
-        <v>438</v>
       </c>
       <c r="AK50" s="33" t="n">
         <v>45658</v>
       </c>
       <c r="AL50" s="32" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="AM50" s="32" t="s">
         <v>422</v>
@@ -11844,7 +11784,7 @@
         <v>45615</v>
       </c>
       <c r="AO50" s="32" t="s">
-        <v>440</v>
+        <v>423</v>
       </c>
       <c r="AP50" s="32" t="s">
         <v>109</v>
@@ -11920,10 +11860,10 @@
       <c r="H51" s="32"/>
       <c r="I51" s="32"/>
       <c r="J51" s="32" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="K51" s="32" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="L51" s="32" t="s">
         <v>128</v>
@@ -11932,10 +11872,10 @@
         <v>233</v>
       </c>
       <c r="N51" s="32" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="O51" s="32" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="P51" s="33" t="n">
         <v>27249</v>
@@ -11970,13 +11910,13 @@
       </c>
       <c r="AI51" s="32"/>
       <c r="AJ51" s="32" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="AK51" s="33" t="n">
         <v>45659</v>
       </c>
       <c r="AL51" s="32" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="AM51" s="32" t="s">
         <v>422</v>
@@ -11985,7 +11925,7 @@
         <v>45615</v>
       </c>
       <c r="AO51" s="32" t="s">
-        <v>447</v>
+        <v>423</v>
       </c>
       <c r="AP51" s="32" t="s">
         <v>109</v>
@@ -12061,10 +12001,10 @@
       <c r="H52" s="32"/>
       <c r="I52" s="32"/>
       <c r="J52" s="32" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="K52" s="32" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="L52" s="32" t="s">
         <v>128</v>
@@ -12073,10 +12013,10 @@
         <v>239</v>
       </c>
       <c r="N52" s="32" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="O52" s="32" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="P52" s="33" t="n">
         <v>37104</v>
@@ -12094,16 +12034,16 @@
         <v>98</v>
       </c>
       <c r="U52" s="32" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="V52" s="33" t="n">
         <v>45613</v>
       </c>
       <c r="W52" s="33" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="X52" s="32" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="Y52" s="33" t="n">
         <v>45613</v>
@@ -12112,7 +12052,7 @@
         <v>252</v>
       </c>
       <c r="AA52" s="32" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="AB52" s="33" t="n">
         <v>45614</v>
@@ -12124,7 +12064,7 @@
       <c r="AE52" s="32"/>
       <c r="AF52" s="32"/>
       <c r="AG52" s="32" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="AH52" s="33" t="n">
         <v>45614</v>
@@ -12133,13 +12073,13 @@
         <v>136</v>
       </c>
       <c r="AJ52" s="32" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="AK52" s="33" t="n">
         <v>45660</v>
       </c>
       <c r="AL52" s="32" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="AM52" s="32" t="s">
         <v>422</v>
@@ -12148,7 +12088,7 @@
         <v>45615</v>
       </c>
       <c r="AO52" s="32" t="s">
-        <v>458</v>
+        <v>423</v>
       </c>
       <c r="AP52" s="32" t="s">
         <v>109</v>
@@ -12224,22 +12164,22 @@
       <c r="H53" s="32"/>
       <c r="I53" s="32"/>
       <c r="J53" s="32" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="K53" s="32" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="L53" s="32" t="s">
         <v>128</v>
       </c>
       <c r="M53" s="32" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="N53" s="32" t="s">
         <v>415</v>
       </c>
       <c r="O53" s="32" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="P53" s="33" t="n">
         <v>34929</v>
@@ -12257,22 +12197,22 @@
         <v>98</v>
       </c>
       <c r="U53" s="32" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="V53" s="33" t="n">
         <v>45610</v>
       </c>
       <c r="W53" s="33" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="X53" s="32" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="Y53" s="33" t="n">
         <v>45610</v>
       </c>
       <c r="Z53" s="33" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="AA53" s="32"/>
       <c r="AB53" s="33"/>
@@ -12281,16 +12221,16 @@
       <c r="AE53" s="32"/>
       <c r="AF53" s="32"/>
       <c r="AG53" s="32" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="AH53" s="33" t="n">
         <v>45610</v>
       </c>
       <c r="AI53" s="33" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="AJ53" s="32" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="AK53" s="33" t="n">
         <v>45661</v>
@@ -12305,7 +12245,7 @@
         <v>45615</v>
       </c>
       <c r="AO53" s="32" t="s">
-        <v>466</v>
+        <v>423</v>
       </c>
       <c r="AP53" s="32" t="s">
         <v>109</v>
@@ -12381,10 +12321,10 @@
       <c r="H54" s="32"/>
       <c r="I54" s="32"/>
       <c r="J54" s="32" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="K54" s="32" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="L54" s="32" t="s">
         <v>128</v>
@@ -12396,7 +12336,7 @@
         <v>303</v>
       </c>
       <c r="O54" s="32" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="P54" s="33" t="n">
         <v>29741</v>
@@ -12414,7 +12354,7 @@
         <v>98</v>
       </c>
       <c r="U54" s="32" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="V54" s="33" t="n">
         <v>45612</v>
@@ -12423,7 +12363,7 @@
         <v>272</v>
       </c>
       <c r="X54" s="32" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="Y54" s="33" t="n">
         <v>45613</v>
@@ -12432,34 +12372,34 @@
         <v>284</v>
       </c>
       <c r="AA54" s="32" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="AB54" s="33" t="n">
         <v>45613</v>
       </c>
       <c r="AC54" s="33" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="AD54" s="32"/>
       <c r="AE54" s="32"/>
       <c r="AF54" s="32"/>
       <c r="AG54" s="32" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="AH54" s="33" t="n">
         <v>45613</v>
       </c>
       <c r="AI54" s="33" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="AJ54" s="32" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="AK54" s="33" t="n">
         <v>45662</v>
       </c>
       <c r="AL54" s="32" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="AM54" s="32" t="s">
         <v>422</v>
@@ -12468,7 +12408,7 @@
         <v>45615</v>
       </c>
       <c r="AO54" s="32" t="s">
-        <v>474</v>
+        <v>423</v>
       </c>
       <c r="AP54" s="32" t="s">
         <v>109</v>
@@ -12544,10 +12484,10 @@
       <c r="H55" s="32"/>
       <c r="I55" s="32"/>
       <c r="J55" s="32" t="s">
-        <v>475</v>
+        <v>469</v>
       </c>
       <c r="K55" s="32" t="s">
-        <v>476</v>
+        <v>470</v>
       </c>
       <c r="L55" s="32" t="s">
         <v>128</v>
@@ -12556,10 +12496,10 @@
         <v>279</v>
       </c>
       <c r="N55" s="32" t="s">
-        <v>477</v>
+        <v>471</v>
       </c>
       <c r="O55" s="32" t="s">
-        <v>478</v>
+        <v>472</v>
       </c>
       <c r="P55" s="33" t="n">
         <v>31350</v>
@@ -12577,7 +12517,7 @@
         <v>98</v>
       </c>
       <c r="U55" s="32" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="V55" s="33" t="n">
         <v>45612</v>
@@ -12586,7 +12526,7 @@
         <v>272</v>
       </c>
       <c r="X55" s="32" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="Y55" s="33" t="n">
         <v>45613</v>
@@ -12595,34 +12535,34 @@
         <v>284</v>
       </c>
       <c r="AA55" s="32" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="AB55" s="33" t="n">
         <v>45613</v>
       </c>
       <c r="AC55" s="33" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="AD55" s="32"/>
       <c r="AE55" s="32"/>
       <c r="AF55" s="32"/>
       <c r="AG55" s="32" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="AH55" s="33" t="n">
         <v>45613</v>
       </c>
       <c r="AI55" s="33" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="AJ55" s="32" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="AK55" s="33" t="n">
         <v>45663</v>
       </c>
       <c r="AL55" s="32" t="s">
-        <v>479</v>
+        <v>473</v>
       </c>
       <c r="AM55" s="32" t="s">
         <v>422</v>
@@ -12631,7 +12571,7 @@
         <v>45615</v>
       </c>
       <c r="AO55" s="32" t="s">
-        <v>480</v>
+        <v>423</v>
       </c>
       <c r="AP55" s="32" t="s">
         <v>109</v>
@@ -12707,10 +12647,10 @@
       <c r="H56" s="32"/>
       <c r="I56" s="32"/>
       <c r="J56" s="32" t="s">
-        <v>481</v>
+        <v>474</v>
       </c>
       <c r="K56" s="32" t="s">
-        <v>482</v>
+        <v>475</v>
       </c>
       <c r="L56" s="32" t="s">
         <v>128</v>
@@ -12722,7 +12662,7 @@
         <v>303</v>
       </c>
       <c r="O56" s="32" t="s">
-        <v>483</v>
+        <v>476</v>
       </c>
       <c r="P56" s="33" t="n">
         <v>25535</v>
@@ -12740,7 +12680,7 @@
         <v>98</v>
       </c>
       <c r="U56" s="32" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="V56" s="33" t="n">
         <v>45612</v>
@@ -12749,7 +12689,7 @@
         <v>272</v>
       </c>
       <c r="X56" s="32" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="Y56" s="33" t="n">
         <v>45613</v>
@@ -12758,34 +12698,34 @@
         <v>284</v>
       </c>
       <c r="AA56" s="32" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="AB56" s="33" t="n">
         <v>45613</v>
       </c>
       <c r="AC56" s="33" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="AD56" s="32"/>
       <c r="AE56" s="32"/>
       <c r="AF56" s="32"/>
       <c r="AG56" s="32" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="AH56" s="33" t="n">
         <v>45613</v>
       </c>
       <c r="AI56" s="33" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="AJ56" s="32" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="AK56" s="33" t="n">
         <v>45664</v>
       </c>
       <c r="AL56" s="32" t="s">
-        <v>484</v>
+        <v>477</v>
       </c>
       <c r="AM56" s="32" t="s">
         <v>422</v>
@@ -12794,7 +12734,7 @@
         <v>45615</v>
       </c>
       <c r="AO56" s="32" t="s">
-        <v>485</v>
+        <v>423</v>
       </c>
       <c r="AP56" s="32" t="s">
         <v>109</v>
@@ -12870,10 +12810,10 @@
       <c r="H57" s="32"/>
       <c r="I57" s="32"/>
       <c r="J57" s="32" t="s">
-        <v>486</v>
+        <v>478</v>
       </c>
       <c r="K57" s="32" t="s">
-        <v>487</v>
+        <v>479</v>
       </c>
       <c r="L57" s="32" t="s">
         <v>128</v>
@@ -12885,7 +12825,7 @@
         <v>314</v>
       </c>
       <c r="O57" s="32" t="s">
-        <v>488</v>
+        <v>480</v>
       </c>
       <c r="P57" s="33" t="n">
         <v>32349</v>
@@ -12903,7 +12843,7 @@
         <v>98</v>
       </c>
       <c r="U57" s="32" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="V57" s="33" t="n">
         <v>45612</v>
@@ -12912,7 +12852,7 @@
         <v>272</v>
       </c>
       <c r="X57" s="32" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="Y57" s="33" t="n">
         <v>45613</v>
@@ -12921,34 +12861,34 @@
         <v>284</v>
       </c>
       <c r="AA57" s="32" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="AB57" s="33" t="n">
         <v>45613</v>
       </c>
       <c r="AC57" s="33" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="AD57" s="32"/>
       <c r="AE57" s="32"/>
       <c r="AF57" s="32"/>
       <c r="AG57" s="32" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="AH57" s="33" t="n">
         <v>45613</v>
       </c>
       <c r="AI57" s="33" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="AJ57" s="32" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="AK57" s="33" t="n">
         <v>45665</v>
       </c>
       <c r="AL57" s="32" t="s">
-        <v>489</v>
+        <v>481</v>
       </c>
       <c r="AM57" s="32" t="s">
         <v>422</v>
@@ -12957,7 +12897,7 @@
         <v>45615</v>
       </c>
       <c r="AO57" s="32" t="s">
-        <v>490</v>
+        <v>482</v>
       </c>
       <c r="AP57" s="32" t="s">
         <v>109</v>
@@ -13033,10 +12973,10 @@
       <c r="H58" s="32"/>
       <c r="I58" s="32"/>
       <c r="J58" s="32" t="s">
-        <v>491</v>
+        <v>483</v>
       </c>
       <c r="K58" s="32" t="s">
-        <v>492</v>
+        <v>484</v>
       </c>
       <c r="L58" s="32" t="s">
         <v>92</v>
@@ -13048,7 +12988,7 @@
         <v>183</v>
       </c>
       <c r="O58" s="32" t="s">
-        <v>493</v>
+        <v>485</v>
       </c>
       <c r="P58" s="33" t="n">
         <v>28254</v>
@@ -13066,7 +13006,7 @@
         <v>98</v>
       </c>
       <c r="U58" s="32" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="V58" s="33" t="n">
         <v>45612</v>
@@ -13075,7 +13015,7 @@
         <v>272</v>
       </c>
       <c r="X58" s="32" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="Y58" s="33" t="n">
         <v>45613</v>
@@ -13084,34 +13024,34 @@
         <v>284</v>
       </c>
       <c r="AA58" s="32" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="AB58" s="33" t="n">
         <v>45613</v>
       </c>
       <c r="AC58" s="33" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="AD58" s="32"/>
       <c r="AE58" s="32"/>
       <c r="AF58" s="32"/>
       <c r="AG58" s="32" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="AH58" s="33" t="n">
         <v>45613</v>
       </c>
       <c r="AI58" s="33" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="AJ58" s="32" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="AK58" s="33" t="n">
         <v>45665</v>
       </c>
       <c r="AL58" s="32" t="s">
-        <v>489</v>
+        <v>481</v>
       </c>
       <c r="AM58" s="32" t="s">
         <v>422</v>
@@ -13120,7 +13060,7 @@
         <v>45615</v>
       </c>
       <c r="AO58" s="32" t="s">
-        <v>494</v>
+        <v>482</v>
       </c>
       <c r="AP58" s="32" t="s">
         <v>109</v>
@@ -13196,22 +13136,22 @@
       <c r="H59" s="32"/>
       <c r="I59" s="32"/>
       <c r="J59" s="32" t="s">
-        <v>495</v>
+        <v>486</v>
       </c>
       <c r="K59" s="32" t="s">
-        <v>496</v>
+        <v>487</v>
       </c>
       <c r="L59" s="32" t="s">
         <v>128</v>
       </c>
       <c r="M59" s="32" t="s">
-        <v>497</v>
+        <v>488</v>
       </c>
       <c r="N59" s="32" t="s">
         <v>415</v>
       </c>
       <c r="O59" s="32" t="s">
-        <v>498</v>
+        <v>489</v>
       </c>
       <c r="P59" s="33" t="n">
         <v>30460</v>
@@ -13229,52 +13169,52 @@
         <v>98</v>
       </c>
       <c r="U59" s="32" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="V59" s="33" t="n">
         <v>45608</v>
       </c>
       <c r="W59" s="33" t="s">
-        <v>499</v>
+        <v>490</v>
       </c>
       <c r="X59" s="32" t="s">
-        <v>500</v>
+        <v>491</v>
       </c>
       <c r="Y59" s="33" t="n">
         <v>45609</v>
       </c>
       <c r="Z59" s="33" t="s">
-        <v>501</v>
+        <v>492</v>
       </c>
       <c r="AA59" s="32" t="s">
-        <v>502</v>
+        <v>493</v>
       </c>
       <c r="AB59" s="33" t="n">
         <v>45609</v>
       </c>
       <c r="AC59" s="33" t="s">
-        <v>503</v>
+        <v>494</v>
       </c>
       <c r="AD59" s="32"/>
       <c r="AE59" s="32"/>
       <c r="AF59" s="32"/>
       <c r="AG59" s="32" t="s">
-        <v>502</v>
+        <v>493</v>
       </c>
       <c r="AH59" s="33" t="n">
         <v>45609</v>
       </c>
       <c r="AI59" s="33" t="s">
-        <v>503</v>
+        <v>494</v>
       </c>
       <c r="AJ59" s="32" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="AK59" s="33" t="n">
         <v>45610</v>
       </c>
       <c r="AL59" s="32" t="s">
-        <v>489</v>
+        <v>481</v>
       </c>
       <c r="AM59" s="32" t="s">
         <v>422</v>
@@ -13283,7 +13223,7 @@
         <v>45615</v>
       </c>
       <c r="AO59" s="32" t="s">
-        <v>504</v>
+        <v>423</v>
       </c>
       <c r="AP59" s="32" t="s">
         <v>109</v>
@@ -13359,22 +13299,22 @@
       <c r="H60" s="32"/>
       <c r="I60" s="32"/>
       <c r="J60" s="32" t="s">
-        <v>505</v>
+        <v>495</v>
       </c>
       <c r="K60" s="32" t="s">
-        <v>506</v>
+        <v>496</v>
       </c>
       <c r="L60" s="32" t="s">
         <v>92</v>
       </c>
       <c r="M60" s="32" t="s">
-        <v>497</v>
+        <v>488</v>
       </c>
       <c r="N60" s="32" t="s">
         <v>415</v>
       </c>
       <c r="O60" s="32" t="s">
-        <v>507</v>
+        <v>497</v>
       </c>
       <c r="P60" s="33" t="n">
         <v>34043</v>
@@ -13392,7 +13332,7 @@
         <v>98</v>
       </c>
       <c r="U60" s="32" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="V60" s="33" t="n">
         <v>45613</v>
@@ -13401,13 +13341,13 @@
         <v>149</v>
       </c>
       <c r="X60" s="32" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="Y60" s="33" t="n">
         <v>45613</v>
       </c>
       <c r="Z60" s="33" t="s">
-        <v>508</v>
+        <v>498</v>
       </c>
       <c r="AA60" s="32"/>
       <c r="AB60" s="33"/>
@@ -13416,22 +13356,22 @@
       <c r="AE60" s="32"/>
       <c r="AF60" s="32"/>
       <c r="AG60" s="32" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="AH60" s="33" t="n">
         <v>45613</v>
       </c>
       <c r="AI60" s="33" t="s">
-        <v>508</v>
+        <v>498</v>
       </c>
       <c r="AJ60" s="32" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="AK60" s="33" t="n">
         <v>45675</v>
       </c>
       <c r="AL60" s="32" t="s">
-        <v>489</v>
+        <v>481</v>
       </c>
       <c r="AM60" s="32" t="s">
         <v>422</v>
@@ -13440,7 +13380,7 @@
         <v>45615</v>
       </c>
       <c r="AO60" s="32" t="s">
-        <v>509</v>
+        <v>423</v>
       </c>
       <c r="AP60" s="32" t="s">
         <v>109</v>
@@ -13516,22 +13456,22 @@
       <c r="H61" s="32"/>
       <c r="I61" s="32"/>
       <c r="J61" s="32" t="s">
-        <v>510</v>
+        <v>499</v>
       </c>
       <c r="K61" s="32" t="s">
-        <v>511</v>
+        <v>500</v>
       </c>
       <c r="L61" s="32" t="s">
         <v>128</v>
       </c>
       <c r="M61" s="32" t="s">
-        <v>497</v>
+        <v>488</v>
       </c>
       <c r="N61" s="32" t="s">
         <v>415</v>
       </c>
       <c r="O61" s="32" t="s">
-        <v>512</v>
+        <v>501</v>
       </c>
       <c r="P61" s="33" t="n">
         <v>34862</v>
@@ -13549,7 +13489,7 @@
         <v>98</v>
       </c>
       <c r="U61" s="32" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="V61" s="33" t="n">
         <v>45613</v>
@@ -13558,7 +13498,7 @@
         <v>149</v>
       </c>
       <c r="X61" s="32" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="Y61" s="33" t="n">
         <v>45614</v>
@@ -13573,7 +13513,7 @@
       <c r="AE61" s="32"/>
       <c r="AF61" s="32"/>
       <c r="AG61" s="32" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="AH61" s="33" t="n">
         <v>45614</v>
@@ -13582,7 +13522,7 @@
         <v>136</v>
       </c>
       <c r="AJ61" s="32" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="AK61" s="33" t="n">
         <v>45675</v>
@@ -13597,7 +13537,7 @@
         <v>45615</v>
       </c>
       <c r="AO61" s="32" t="s">
-        <v>513</v>
+        <v>423</v>
       </c>
       <c r="AP61" s="32" t="s">
         <v>109</v>
@@ -13673,10 +13613,10 @@
       <c r="H62" s="32"/>
       <c r="I62" s="32"/>
       <c r="J62" s="32" t="s">
-        <v>514</v>
+        <v>502</v>
       </c>
       <c r="K62" s="32" t="s">
-        <v>515</v>
+        <v>503</v>
       </c>
       <c r="L62" s="32" t="s">
         <v>128</v>
@@ -13688,7 +13628,7 @@
         <v>210</v>
       </c>
       <c r="O62" s="32" t="s">
-        <v>516</v>
+        <v>504</v>
       </c>
       <c r="P62" s="33" t="n">
         <v>29744</v>
@@ -13706,16 +13646,16 @@
         <v>98</v>
       </c>
       <c r="U62" s="32" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="V62" s="33" t="n">
         <v>45613</v>
       </c>
       <c r="W62" s="33" t="s">
-        <v>517</v>
+        <v>505</v>
       </c>
       <c r="X62" s="32" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="Y62" s="33" t="n">
         <v>45613</v>
@@ -13724,28 +13664,28 @@
         <v>102</v>
       </c>
       <c r="AA62" s="32" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="AB62" s="33" t="n">
         <v>45613</v>
       </c>
       <c r="AC62" s="33" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="AD62" s="32"/>
       <c r="AE62" s="32"/>
       <c r="AF62" s="32"/>
       <c r="AG62" s="32" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="AH62" s="33" t="n">
         <v>45613</v>
       </c>
       <c r="AI62" s="33" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="AJ62" s="32" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="AK62" s="33" t="n">
         <v>45675</v>
@@ -13760,7 +13700,7 @@
         <v>45615</v>
       </c>
       <c r="AO62" s="32" t="s">
-        <v>518</v>
+        <v>423</v>
       </c>
       <c r="AP62" s="32" t="s">
         <v>109</v>
@@ -13836,22 +13776,22 @@
       <c r="H63" s="32"/>
       <c r="I63" s="32"/>
       <c r="J63" s="32" t="s">
-        <v>519</v>
+        <v>506</v>
       </c>
       <c r="K63" s="32" t="s">
-        <v>520</v>
+        <v>507</v>
       </c>
       <c r="L63" s="32" t="s">
         <v>92</v>
       </c>
       <c r="M63" s="32" t="s">
-        <v>521</v>
+        <v>508</v>
       </c>
       <c r="N63" s="32" t="s">
         <v>415</v>
       </c>
       <c r="O63" s="32" t="s">
-        <v>522</v>
+        <v>509</v>
       </c>
       <c r="P63" s="33" t="n">
         <v>26701</v>
@@ -13869,13 +13809,13 @@
         <v>98</v>
       </c>
       <c r="U63" s="32" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="V63" s="33" t="n">
         <v>45609</v>
       </c>
       <c r="W63" s="33" t="s">
-        <v>523</v>
+        <v>510</v>
       </c>
       <c r="X63" s="32" t="s">
         <v>285</v>
@@ -13884,7 +13824,7 @@
         <v>45609</v>
       </c>
       <c r="Z63" s="33" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="AA63" s="32"/>
       <c r="AB63" s="33"/>
@@ -13899,16 +13839,16 @@
         <v>45609</v>
       </c>
       <c r="AI63" s="33" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="AJ63" s="32" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="AK63" s="33" t="n">
         <v>45610</v>
       </c>
       <c r="AL63" s="32" t="s">
-        <v>524</v>
+        <v>511</v>
       </c>
       <c r="AM63" s="32" t="s">
         <v>422</v>
@@ -13917,7 +13857,7 @@
         <v>45615</v>
       </c>
       <c r="AO63" s="32" t="s">
-        <v>525</v>
+        <v>423</v>
       </c>
       <c r="AP63" s="32" t="s">
         <v>109</v>
@@ -13993,31 +13933,31 @@
       <c r="H64" s="32"/>
       <c r="I64" s="32"/>
       <c r="J64" s="32" t="s">
-        <v>526</v>
+        <v>512</v>
       </c>
       <c r="K64" s="32" t="s">
-        <v>527</v>
+        <v>513</v>
       </c>
       <c r="L64" s="32" t="s">
         <v>128</v>
       </c>
       <c r="M64" s="32" t="s">
-        <v>528</v>
+        <v>514</v>
       </c>
       <c r="N64" s="32" t="s">
         <v>143</v>
       </c>
       <c r="O64" s="32" t="s">
-        <v>529</v>
+        <v>515</v>
       </c>
       <c r="P64" s="33" t="n">
         <v>24200</v>
       </c>
       <c r="Q64" s="32" t="s">
-        <v>530</v>
+        <v>516</v>
       </c>
       <c r="R64" s="32" t="s">
-        <v>530</v>
+        <v>516</v>
       </c>
       <c r="S64" s="32" t="s">
         <v>98</v>
@@ -14026,16 +13966,16 @@
         <v>98</v>
       </c>
       <c r="U64" s="32" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="V64" s="33" t="n">
         <v>45613</v>
       </c>
       <c r="W64" s="33" t="s">
-        <v>531</v>
+        <v>517</v>
       </c>
       <c r="X64" s="32" t="s">
-        <v>532</v>
+        <v>518</v>
       </c>
       <c r="Y64" s="33" t="n">
         <v>45613</v>
@@ -14050,7 +13990,7 @@
       <c r="AE64" s="32"/>
       <c r="AF64" s="32"/>
       <c r="AG64" s="32" t="s">
-        <v>532</v>
+        <v>518</v>
       </c>
       <c r="AH64" s="33" t="n">
         <v>45613</v>
@@ -14059,7 +13999,7 @@
         <v>420</v>
       </c>
       <c r="AJ64" s="32" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="AK64" s="33" t="n">
         <v>45675</v>
@@ -14074,7 +14014,7 @@
         <v>45615</v>
       </c>
       <c r="AO64" s="32" t="s">
-        <v>533</v>
+        <v>423</v>
       </c>
       <c r="AP64" s="32" t="s">
         <v>109</v>
@@ -14150,58 +14090,58 @@
       <c r="H65" s="32"/>
       <c r="I65" s="32"/>
       <c r="J65" s="32" t="s">
-        <v>534</v>
+        <v>519</v>
       </c>
       <c r="K65" s="32" t="s">
-        <v>535</v>
+        <v>520</v>
       </c>
       <c r="L65" s="32" t="s">
         <v>128</v>
       </c>
       <c r="M65" s="32" t="s">
-        <v>528</v>
+        <v>514</v>
       </c>
       <c r="N65" s="32" t="s">
-        <v>536</v>
+        <v>521</v>
       </c>
       <c r="O65" s="32" t="s">
-        <v>537</v>
+        <v>522</v>
       </c>
       <c r="P65" s="33" t="n">
         <v>29879</v>
       </c>
       <c r="Q65" s="32" t="s">
-        <v>538</v>
+        <v>523</v>
       </c>
       <c r="R65" s="32" t="s">
-        <v>530</v>
+        <v>516</v>
       </c>
       <c r="S65" s="32" t="s">
-        <v>530</v>
+        <v>516</v>
       </c>
       <c r="T65" s="32" t="s">
         <v>98</v>
       </c>
       <c r="U65" s="32" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="V65" s="33" t="n">
         <v>45613</v>
       </c>
       <c r="W65" s="33" t="s">
-        <v>539</v>
+        <v>524</v>
       </c>
       <c r="X65" s="32" t="s">
-        <v>540</v>
+        <v>525</v>
       </c>
       <c r="Y65" s="33" t="n">
         <v>45613</v>
       </c>
       <c r="Z65" s="33" t="s">
-        <v>541</v>
+        <v>526</v>
       </c>
       <c r="AA65" s="32" t="s">
-        <v>532</v>
+        <v>518</v>
       </c>
       <c r="AB65" s="33" t="n">
         <v>45613</v>
@@ -14213,7 +14153,7 @@
       <c r="AE65" s="32"/>
       <c r="AF65" s="32"/>
       <c r="AG65" s="32" t="s">
-        <v>532</v>
+        <v>518</v>
       </c>
       <c r="AH65" s="33" t="n">
         <v>45613</v>
@@ -14222,7 +14162,7 @@
         <v>420</v>
       </c>
       <c r="AJ65" s="32" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="AK65" s="33" t="n">
         <v>45675</v>
@@ -14237,7 +14177,7 @@
         <v>45615</v>
       </c>
       <c r="AO65" s="32" t="s">
-        <v>542</v>
+        <v>482</v>
       </c>
       <c r="AP65" s="32" t="s">
         <v>109</v>
@@ -14313,28 +14253,28 @@
       <c r="H66" s="32"/>
       <c r="I66" s="32"/>
       <c r="J66" s="32" t="s">
-        <v>543</v>
+        <v>527</v>
       </c>
       <c r="K66" s="32" t="s">
-        <v>544</v>
+        <v>528</v>
       </c>
       <c r="L66" s="32" t="s">
         <v>128</v>
       </c>
       <c r="M66" s="32" t="s">
-        <v>528</v>
+        <v>514</v>
       </c>
       <c r="N66" s="32" t="s">
-        <v>545</v>
+        <v>529</v>
       </c>
       <c r="O66" s="32" t="s">
-        <v>546</v>
+        <v>530</v>
       </c>
       <c r="P66" s="33" t="n">
         <v>28476</v>
       </c>
       <c r="Q66" s="32" t="s">
-        <v>538</v>
+        <v>523</v>
       </c>
       <c r="R66" s="32" t="s">
         <v>97</v>
@@ -14346,46 +14286,46 @@
         <v>98</v>
       </c>
       <c r="U66" s="32" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="V66" s="33" t="n">
         <v>45613</v>
       </c>
       <c r="W66" s="33" t="s">
-        <v>547</v>
+        <v>531</v>
       </c>
       <c r="X66" s="32" t="s">
-        <v>540</v>
+        <v>525</v>
       </c>
       <c r="Y66" s="33" t="n">
         <v>45613</v>
       </c>
       <c r="Z66" s="33" t="s">
-        <v>548</v>
+        <v>532</v>
       </c>
       <c r="AA66" s="32" t="s">
-        <v>532</v>
+        <v>518</v>
       </c>
       <c r="AB66" s="33" t="n">
         <v>45614</v>
       </c>
       <c r="AC66" s="33" t="s">
-        <v>549</v>
+        <v>533</v>
       </c>
       <c r="AD66" s="32"/>
       <c r="AE66" s="32"/>
       <c r="AF66" s="32"/>
       <c r="AG66" s="32" t="s">
-        <v>532</v>
+        <v>518</v>
       </c>
       <c r="AH66" s="33" t="n">
         <v>45614</v>
       </c>
       <c r="AI66" s="33" t="s">
-        <v>549</v>
+        <v>533</v>
       </c>
       <c r="AJ66" s="32" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="AK66" s="33" t="n">
         <v>45675</v>
@@ -14400,7 +14340,7 @@
         <v>45615</v>
       </c>
       <c r="AO66" s="32" t="s">
-        <v>550</v>
+        <v>423</v>
       </c>
       <c r="AP66" s="32" t="s">
         <v>109</v>
@@ -14476,22 +14416,22 @@
       <c r="H67" s="32"/>
       <c r="I67" s="32"/>
       <c r="J67" s="32" t="s">
-        <v>551</v>
+        <v>534</v>
       </c>
       <c r="K67" s="32" t="s">
-        <v>552</v>
+        <v>535</v>
       </c>
       <c r="L67" s="32" t="s">
         <v>92</v>
       </c>
       <c r="M67" s="32" t="s">
-        <v>553</v>
+        <v>536</v>
       </c>
       <c r="N67" s="32" t="s">
-        <v>554</v>
+        <v>537</v>
       </c>
       <c r="O67" s="32" t="s">
-        <v>555</v>
+        <v>538</v>
       </c>
       <c r="P67" s="33" t="n">
         <v>28646</v>
@@ -14509,22 +14449,22 @@
         <v>98</v>
       </c>
       <c r="U67" s="32" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="V67" s="33" t="n">
         <v>45613</v>
       </c>
       <c r="W67" s="33" t="s">
-        <v>556</v>
+        <v>539</v>
       </c>
       <c r="X67" s="32" t="s">
-        <v>540</v>
+        <v>525</v>
       </c>
       <c r="Y67" s="33" t="n">
         <v>45614</v>
       </c>
       <c r="Z67" s="33" t="s">
-        <v>557</v>
+        <v>540</v>
       </c>
       <c r="AA67" s="32"/>
       <c r="AB67" s="33"/>
@@ -14533,16 +14473,16 @@
       <c r="AE67" s="32"/>
       <c r="AF67" s="32"/>
       <c r="AG67" s="32" t="s">
-        <v>540</v>
+        <v>525</v>
       </c>
       <c r="AH67" s="33" t="n">
         <v>45614</v>
       </c>
       <c r="AI67" s="33" t="s">
-        <v>557</v>
+        <v>540</v>
       </c>
       <c r="AJ67" s="32" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="AK67" s="33" t="n">
         <v>45675</v>
@@ -14557,7 +14497,7 @@
         <v>45615</v>
       </c>
       <c r="AO67" s="32" t="s">
-        <v>558</v>
+        <v>423</v>
       </c>
       <c r="AP67" s="32" t="s">
         <v>109</v>
@@ -14633,31 +14573,31 @@
       <c r="H68" s="32"/>
       <c r="I68" s="32"/>
       <c r="J68" s="32" t="s">
-        <v>559</v>
+        <v>541</v>
       </c>
       <c r="K68" s="32" t="s">
-        <v>560</v>
+        <v>542</v>
       </c>
       <c r="L68" s="32" t="s">
         <v>92</v>
       </c>
       <c r="M68" s="32" t="s">
-        <v>553</v>
+        <v>536</v>
       </c>
       <c r="N68" s="32" t="s">
         <v>415</v>
       </c>
       <c r="O68" s="32" t="s">
-        <v>561</v>
+        <v>543</v>
       </c>
       <c r="P68" s="33" t="n">
         <v>34573</v>
       </c>
       <c r="Q68" s="32" t="s">
-        <v>530</v>
+        <v>516</v>
       </c>
       <c r="R68" s="32" t="s">
-        <v>530</v>
+        <v>516</v>
       </c>
       <c r="S68" s="32" t="s">
         <v>98</v>
@@ -14666,16 +14606,16 @@
         <v>98</v>
       </c>
       <c r="U68" s="32" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="V68" s="33" t="n">
         <v>45609</v>
       </c>
       <c r="W68" s="33" t="s">
-        <v>562</v>
+        <v>544</v>
       </c>
       <c r="X68" s="32" t="s">
-        <v>532</v>
+        <v>518</v>
       </c>
       <c r="Y68" s="33" t="n">
         <v>45609</v>
@@ -14690,7 +14630,7 @@
       <c r="AE68" s="32"/>
       <c r="AF68" s="32"/>
       <c r="AG68" s="32" t="s">
-        <v>532</v>
+        <v>518</v>
       </c>
       <c r="AH68" s="33" t="n">
         <v>45609</v>
@@ -14699,13 +14639,13 @@
         <v>420</v>
       </c>
       <c r="AJ68" s="32" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="AK68" s="33" t="n">
         <v>45610</v>
       </c>
       <c r="AL68" s="32" t="s">
-        <v>524</v>
+        <v>511</v>
       </c>
       <c r="AM68" s="32" t="s">
         <v>422</v>
@@ -14714,7 +14654,7 @@
         <v>45615</v>
       </c>
       <c r="AO68" s="32" t="s">
-        <v>563</v>
+        <v>423</v>
       </c>
       <c r="AP68" s="32" t="s">
         <v>109</v>
@@ -14790,28 +14730,28 @@
       <c r="H69" s="32"/>
       <c r="I69" s="32"/>
       <c r="J69" s="32" t="s">
-        <v>564</v>
+        <v>545</v>
       </c>
       <c r="K69" s="32" t="s">
-        <v>565</v>
+        <v>546</v>
       </c>
       <c r="L69" s="32" t="s">
         <v>128</v>
       </c>
       <c r="M69" s="32" t="s">
-        <v>566</v>
+        <v>547</v>
       </c>
       <c r="N69" s="32" t="s">
         <v>415</v>
       </c>
       <c r="O69" s="32" t="s">
-        <v>567</v>
+        <v>548</v>
       </c>
       <c r="P69" s="33" t="n">
         <v>29004</v>
       </c>
       <c r="Q69" s="32" t="s">
-        <v>568</v>
+        <v>549</v>
       </c>
       <c r="R69" s="32" t="s">
         <v>96</v>
@@ -14823,58 +14763,58 @@
         <v>97</v>
       </c>
       <c r="U69" s="32" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="V69" s="33" t="n">
         <v>45608</v>
       </c>
       <c r="W69" s="33" t="s">
-        <v>569</v>
+        <v>550</v>
       </c>
       <c r="X69" s="32" t="s">
-        <v>570</v>
+        <v>551</v>
       </c>
       <c r="Y69" s="33" t="n">
         <v>45608</v>
       </c>
       <c r="Z69" s="33" t="s">
-        <v>571</v>
+        <v>552</v>
       </c>
       <c r="AA69" s="32" t="s">
-        <v>572</v>
+        <v>553</v>
       </c>
       <c r="AB69" s="33" t="n">
         <v>45609</v>
       </c>
       <c r="AC69" s="33" t="s">
-        <v>573</v>
+        <v>554</v>
       </c>
       <c r="AD69" s="32" t="s">
-        <v>574</v>
+        <v>555</v>
       </c>
       <c r="AE69" s="33" t="n">
         <v>45609</v>
       </c>
       <c r="AF69" s="32" t="s">
-        <v>575</v>
+        <v>556</v>
       </c>
       <c r="AG69" s="32" t="s">
-        <v>574</v>
+        <v>555</v>
       </c>
       <c r="AH69" s="33" t="n">
         <v>45609</v>
       </c>
       <c r="AI69" s="32" t="s">
-        <v>575</v>
+        <v>556</v>
       </c>
       <c r="AJ69" s="32" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="AK69" s="33" t="n">
         <v>45610</v>
       </c>
       <c r="AL69" s="32" t="s">
-        <v>524</v>
+        <v>511</v>
       </c>
       <c r="AM69" s="32" t="s">
         <v>422</v>
@@ -14883,7 +14823,7 @@
         <v>45615</v>
       </c>
       <c r="AO69" s="32" t="s">
-        <v>576</v>
+        <v>423</v>
       </c>
       <c r="AP69" s="32" t="s">
         <v>109</v>
@@ -15477,7 +15417,7 @@
   <dimension ref="A1:BV5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="W5" activeCellId="0" sqref="W5"/>
+      <selection pane="topLeft" activeCell="W5" activeCellId="1" sqref="AO48 W5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15563,7 +15503,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="28" t="s">
-        <v>577</v>
+        <v>557</v>
       </c>
       <c r="D1" s="28" t="s">
         <v>3</v>
@@ -15572,13 +15512,13 @@
         <v>4</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>578</v>
+        <v>558</v>
       </c>
       <c r="G1" s="10" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>579</v>
+        <v>559</v>
       </c>
       <c r="I1" s="12" t="s">
         <v>8</v>
@@ -15802,28 +15742,28 @@
         <v>125</v>
       </c>
       <c r="H2" s="32" t="s">
-        <v>580</v>
+        <v>560</v>
       </c>
       <c r="I2" s="32" t="s">
-        <v>580</v>
+        <v>560</v>
       </c>
       <c r="J2" s="32" t="s">
-        <v>581</v>
+        <v>561</v>
       </c>
       <c r="K2" s="32" t="s">
-        <v>582</v>
+        <v>562</v>
       </c>
       <c r="L2" s="32" t="s">
         <v>128</v>
       </c>
       <c r="M2" s="32" t="s">
-        <v>583</v>
+        <v>563</v>
       </c>
       <c r="N2" s="32" t="s">
         <v>143</v>
       </c>
       <c r="O2" s="32" t="s">
-        <v>584</v>
+        <v>564</v>
       </c>
       <c r="P2" s="33" t="n">
         <v>36506</v>
@@ -15833,13 +15773,13 @@
       <c r="S2" s="32"/>
       <c r="T2" s="32"/>
       <c r="U2" s="32" t="s">
-        <v>585</v>
+        <v>565</v>
       </c>
       <c r="V2" s="32" t="s">
-        <v>586</v>
+        <v>566</v>
       </c>
       <c r="W2" s="32" t="s">
-        <v>587</v>
+        <v>567</v>
       </c>
       <c r="X2" s="32"/>
       <c r="Y2" s="32"/>
@@ -15895,10 +15835,10 @@
     </row>
     <row r="3" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="32" t="s">
-        <v>588</v>
+        <v>568</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>589</v>
+        <v>569</v>
       </c>
       <c r="C3" s="33" t="n">
         <v>45569</v>
@@ -15916,34 +15856,34 @@
         <v>89</v>
       </c>
       <c r="H3" s="32" t="s">
-        <v>580</v>
+        <v>560</v>
       </c>
       <c r="I3" s="32" t="s">
-        <v>580</v>
+        <v>560</v>
       </c>
       <c r="J3" s="32" t="s">
-        <v>590</v>
+        <v>570</v>
       </c>
       <c r="K3" s="32" t="s">
-        <v>591</v>
+        <v>571</v>
       </c>
       <c r="L3" s="32" t="s">
         <v>128</v>
       </c>
       <c r="M3" s="32" t="s">
-        <v>583</v>
+        <v>563</v>
       </c>
       <c r="N3" s="32" t="s">
         <v>143</v>
       </c>
       <c r="O3" s="32" t="s">
-        <v>592</v>
+        <v>572</v>
       </c>
       <c r="P3" s="33" t="n">
         <v>24829</v>
       </c>
       <c r="Q3" s="32" t="s">
-        <v>593</v>
+        <v>573</v>
       </c>
       <c r="R3" s="32"/>
       <c r="S3" s="32"/>
@@ -15958,22 +15898,22 @@
         <v>108</v>
       </c>
       <c r="X3" s="32" t="s">
-        <v>594</v>
+        <v>574</v>
       </c>
       <c r="Y3" s="33" t="n">
         <v>45557</v>
       </c>
       <c r="Z3" s="32" t="s">
-        <v>595</v>
+        <v>575</v>
       </c>
       <c r="AA3" s="32" t="s">
-        <v>596</v>
+        <v>576</v>
       </c>
       <c r="AB3" s="49" t="n">
         <v>45557</v>
       </c>
       <c r="AC3" s="32" t="s">
-        <v>597</v>
+        <v>577</v>
       </c>
       <c r="AD3" s="32" t="s">
         <v>109</v>
@@ -15988,7 +15928,7 @@
         <v>2</v>
       </c>
       <c r="AH3" s="32" t="s">
-        <v>598</v>
+        <v>578</v>
       </c>
       <c r="AI3" s="49" t="n">
         <v>45557</v>
@@ -15997,13 +15937,13 @@
         <v>45558</v>
       </c>
       <c r="AK3" s="32" t="s">
-        <v>599</v>
+        <v>579</v>
       </c>
       <c r="AL3" s="32" t="s">
-        <v>600</v>
+        <v>580</v>
       </c>
       <c r="AM3" s="32" t="s">
-        <v>601</v>
+        <v>581</v>
       </c>
       <c r="AN3" s="49" t="n">
         <v>45557</v>
@@ -16012,10 +15952,10 @@
         <v>45558</v>
       </c>
       <c r="AP3" s="32" t="s">
-        <v>599</v>
+        <v>579</v>
       </c>
       <c r="AQ3" s="32" t="s">
-        <v>602</v>
+        <v>582</v>
       </c>
       <c r="AR3" s="32" t="s">
         <v>115</v>
@@ -16027,10 +15967,10 @@
         <v>45558</v>
       </c>
       <c r="AU3" s="32" t="s">
-        <v>599</v>
+        <v>579</v>
       </c>
       <c r="AV3" s="32" t="s">
-        <v>603</v>
+        <v>583</v>
       </c>
       <c r="AW3" s="32" t="s">
         <v>117</v>
@@ -16069,7 +16009,7 @@
         <v>45557</v>
       </c>
       <c r="BI3" s="32" t="s">
-        <v>604</v>
+        <v>584</v>
       </c>
       <c r="BJ3" s="32" t="s">
         <v>244</v>
@@ -16081,7 +16021,7 @@
         <v>45557</v>
       </c>
       <c r="BM3" s="32" t="s">
-        <v>604</v>
+        <v>584</v>
       </c>
       <c r="BN3" s="32" t="s">
         <v>244</v>
@@ -16093,16 +16033,16 @@
         <v>45557</v>
       </c>
       <c r="BQ3" s="32" t="s">
-        <v>604</v>
+        <v>584</v>
       </c>
       <c r="BR3" s="32" t="s">
-        <v>605</v>
+        <v>585</v>
       </c>
       <c r="BS3" s="32" t="s">
         <v>122</v>
       </c>
       <c r="BT3" s="32" t="s">
-        <v>606</v>
+        <v>586</v>
       </c>
       <c r="BU3" s="49" t="n">
         <v>45557</v>
@@ -16113,10 +16053,10 @@
     </row>
     <row r="4" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="32" t="s">
-        <v>607</v>
+        <v>587</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>608</v>
+        <v>588</v>
       </c>
       <c r="C4" s="33" t="n">
         <v>45918</v>
@@ -16128,33 +16068,33 @@
         <v>45918</v>
       </c>
       <c r="F4" s="32" t="s">
-        <v>609</v>
+        <v>589</v>
       </c>
       <c r="G4" s="32" t="s">
-        <v>610</v>
+        <v>590</v>
       </c>
       <c r="H4" s="32"/>
       <c r="I4" s="32"/>
       <c r="J4" s="32" t="s">
-        <v>611</v>
+        <v>591</v>
       </c>
       <c r="K4" s="32" t="s">
-        <v>612</v>
+        <v>592</v>
       </c>
       <c r="L4" s="32" t="s">
         <v>92</v>
       </c>
       <c r="M4" s="32" t="s">
-        <v>613</v>
+        <v>593</v>
       </c>
       <c r="N4" s="32" t="s">
-        <v>614</v>
+        <v>594</v>
       </c>
       <c r="O4" s="32" t="s">
-        <v>615</v>
+        <v>595</v>
       </c>
       <c r="P4" s="33" t="s">
-        <v>616</v>
+        <v>596</v>
       </c>
       <c r="Q4" s="32"/>
       <c r="R4" s="32"/>
@@ -16167,16 +16107,16 @@
         <v>45611</v>
       </c>
       <c r="W4" s="32" t="s">
-        <v>617</v>
+        <v>597</v>
       </c>
       <c r="X4" s="32" t="s">
-        <v>594</v>
+        <v>574</v>
       </c>
       <c r="Y4" s="33" t="n">
         <v>45558</v>
       </c>
       <c r="Z4" s="32" t="s">
-        <v>618</v>
+        <v>598</v>
       </c>
       <c r="AA4" s="32"/>
       <c r="AB4" s="32"/>
@@ -16226,7 +16166,7 @@
       <c r="BR4" s="32"/>
       <c r="BS4" s="32"/>
       <c r="BT4" s="32" t="s">
-        <v>619</v>
+        <v>599</v>
       </c>
       <c r="BU4" s="32"/>
       <c r="BV4" s="32" t="s">

</xml_diff>

<commit_message>
Reporte Hoteles Listo, roomlist ajustado
</commit_message>
<xml_diff>
--- a/ejemplo_carga_masiva.xlsx
+++ b/ejemplo_carga_masiva.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2425" uniqueCount="592">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2427" uniqueCount="592">
   <si>
     <t xml:space="preserve">Owner</t>
   </si>
@@ -2359,8 +2359,8 @@
   </sheetPr>
   <dimension ref="A1:CH75"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AE1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AJ38" activeCellId="0" sqref="AJ38:AL38"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AP1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="BA10" activeCellId="0" sqref="BA10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2843,10 +2843,10 @@
         <v>112</v>
       </c>
       <c r="AU2" s="33" t="n">
-        <v>45610</v>
+        <v>45611</v>
       </c>
       <c r="AV2" s="33" t="n">
-        <v>45611</v>
+        <v>45612</v>
       </c>
       <c r="AW2" s="32" t="s">
         <v>113</v>
@@ -3057,10 +3057,10 @@
         <v>112</v>
       </c>
       <c r="AU3" s="33" t="n">
-        <v>45610</v>
+        <v>45611</v>
       </c>
       <c r="AV3" s="33" t="n">
-        <v>45611</v>
+        <v>45612</v>
       </c>
       <c r="AW3" s="32" t="s">
         <v>139</v>
@@ -3441,10 +3441,10 @@
         <v>112</v>
       </c>
       <c r="AU5" s="33" t="n">
-        <v>45610</v>
+        <v>45611</v>
       </c>
       <c r="AV5" s="33" t="n">
-        <v>45611</v>
+        <v>45612</v>
       </c>
       <c r="AW5" s="32" t="s">
         <v>169</v>
@@ -3658,7 +3658,7 @@
         <v>45611</v>
       </c>
       <c r="AV6" s="33" t="n">
-        <v>45611</v>
+        <v>45612</v>
       </c>
       <c r="AW6" s="32"/>
       <c r="AX6" s="32" t="s">
@@ -3861,7 +3861,7 @@
         <v>45611</v>
       </c>
       <c r="AV7" s="33" t="n">
-        <v>45611</v>
+        <v>45612</v>
       </c>
       <c r="AW7" s="32"/>
       <c r="AX7" s="32" t="s">
@@ -4064,7 +4064,7 @@
         <v>45611</v>
       </c>
       <c r="AV8" s="33" t="n">
-        <v>45611</v>
+        <v>45612</v>
       </c>
       <c r="AW8" s="32"/>
       <c r="AX8" s="32" t="s">
@@ -4264,10 +4264,10 @@
         <v>112</v>
       </c>
       <c r="AU9" s="33" t="n">
-        <v>45610</v>
+        <v>45611</v>
       </c>
       <c r="AV9" s="33" t="n">
-        <v>45611</v>
+        <v>45612</v>
       </c>
       <c r="AW9" s="32" t="s">
         <v>139</v>
@@ -4488,10 +4488,10 @@
         <v>112</v>
       </c>
       <c r="AU10" s="33" t="n">
-        <v>45610</v>
+        <v>45611</v>
       </c>
       <c r="AV10" s="33" t="n">
-        <v>45611</v>
+        <v>45612</v>
       </c>
       <c r="AW10" s="32" t="s">
         <v>139</v>
@@ -4704,7 +4704,7 @@
         <v>45611</v>
       </c>
       <c r="AV11" s="33" t="n">
-        <v>45611</v>
+        <v>45612</v>
       </c>
       <c r="AW11" s="32"/>
       <c r="AX11" s="32" t="s">
@@ -4897,7 +4897,7 @@
         <v>45611</v>
       </c>
       <c r="AV12" s="33" t="n">
-        <v>45611</v>
+        <v>45612</v>
       </c>
       <c r="AW12" s="32"/>
       <c r="AX12" s="32" t="s">
@@ -5090,7 +5090,7 @@
         <v>45611</v>
       </c>
       <c r="AV13" s="33" t="n">
-        <v>45611</v>
+        <v>45612</v>
       </c>
       <c r="AW13" s="32"/>
       <c r="AX13" s="32" t="s">
@@ -5283,7 +5283,7 @@
         <v>45611</v>
       </c>
       <c r="AV14" s="33" t="n">
-        <v>45611</v>
+        <v>45612</v>
       </c>
       <c r="AW14" s="32"/>
       <c r="AX14" s="32" t="s">
@@ -5476,7 +5476,7 @@
         <v>45611</v>
       </c>
       <c r="AV15" s="33" t="n">
-        <v>45611</v>
+        <v>45612</v>
       </c>
       <c r="AW15" s="32"/>
       <c r="AX15" s="32" t="s">
@@ -5666,10 +5666,10 @@
         <v>112</v>
       </c>
       <c r="AU16" s="33" t="n">
-        <v>45610</v>
+        <v>45611</v>
       </c>
       <c r="AV16" s="33" t="n">
-        <v>45611</v>
+        <v>45612</v>
       </c>
       <c r="AW16" s="32" t="s">
         <v>153</v>
@@ -15392,8 +15392,8 @@
   </sheetPr>
   <dimension ref="A1:BV5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="W5" activeCellId="1" sqref="AJ38:AL38 W5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AJ3" activeCellId="0" sqref="AJ3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15907,10 +15907,10 @@
         <v>570</v>
       </c>
       <c r="AI3" s="49" t="n">
-        <v>45557</v>
+        <v>45570</v>
       </c>
       <c r="AJ3" s="49" t="n">
-        <v>45558</v>
+        <v>45571</v>
       </c>
       <c r="AK3" s="32" t="s">
         <v>571</v>
@@ -15922,10 +15922,10 @@
         <v>573</v>
       </c>
       <c r="AN3" s="49" t="n">
-        <v>45557</v>
+        <v>45571</v>
       </c>
       <c r="AO3" s="49" t="n">
-        <v>45558</v>
+        <v>45572</v>
       </c>
       <c r="AP3" s="32" t="s">
         <v>571</v>
@@ -15937,10 +15937,10 @@
         <v>115</v>
       </c>
       <c r="AS3" s="49" t="n">
-        <v>45557</v>
+        <v>45573</v>
       </c>
       <c r="AT3" s="49" t="n">
-        <v>45558</v>
+        <v>45574</v>
       </c>
       <c r="AU3" s="32" t="s">
         <v>571</v>
@@ -16127,10 +16127,18 @@
       <c r="BE4" s="32" t="s">
         <v>186</v>
       </c>
-      <c r="BF4" s="32"/>
-      <c r="BG4" s="32"/>
-      <c r="BH4" s="32"/>
-      <c r="BI4" s="32"/>
+      <c r="BF4" s="32" t="s">
+        <v>205</v>
+      </c>
+      <c r="BG4" s="49" t="n">
+        <v>45587</v>
+      </c>
+      <c r="BH4" s="49" t="n">
+        <v>45587</v>
+      </c>
+      <c r="BI4" s="32" t="s">
+        <v>214</v>
+      </c>
       <c r="BJ4" s="32"/>
       <c r="BK4" s="32"/>
       <c r="BL4" s="32"/>

</xml_diff>